<commit_message>
Release Demons of Decay
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5936ABE7-C3A1-415A-9E29-EDEBA3EEB7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD4BCBB-609F-4407-B008-3FADBB279579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="312">
   <si>
     <t>Name</t>
   </si>
@@ -715,9 +715,6 @@
     <t>Cost(gp)</t>
   </si>
   <si>
-    <t>Requirement</t>
-  </si>
-  <si>
     <t># of Effects</t>
   </si>
   <si>
@@ -745,6 +742,9 @@
     <t>Fireworks</t>
   </si>
   <si>
+    <t>Trolls</t>
+  </si>
+  <si>
     <t>Player Race: Trolls</t>
   </si>
   <si>
@@ -878,13 +878,136 @@
   </si>
   <si>
     <t>Witstealer Sword</t>
+  </si>
+  <si>
+    <t>Tigers</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Dire Tiger</t>
+  </si>
+  <si>
+    <t>Weretiger</t>
+  </si>
+  <si>
+    <t>Equation Master</t>
+  </si>
+  <si>
+    <t>Material Master</t>
+  </si>
+  <si>
+    <t>Scroll Master</t>
+  </si>
+  <si>
+    <t>Somatic Master</t>
+  </si>
+  <si>
+    <t>Verbal Master</t>
+  </si>
+  <si>
+    <t>Prerequisite</t>
+  </si>
+  <si>
+    <t>A spellcasting feature that grants spell slots</t>
+  </si>
+  <si>
+    <t>The ability to cast at least one spell</t>
+  </si>
+  <si>
+    <t>The ability to use spell scrolls</t>
+  </si>
+  <si>
+    <t>Acid Rain</t>
+  </si>
+  <si>
+    <t>Evocation</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Acid Wave</t>
+  </si>
+  <si>
+    <t>Bolt of Change</t>
+  </si>
+  <si>
+    <t>Trasmutation</t>
+  </si>
+  <si>
+    <t>Cacophonic Caress</t>
+  </si>
+  <si>
+    <t>Chaos Storm</t>
+  </si>
+  <si>
+    <t>Frost Nova</t>
+  </si>
+  <si>
+    <t>Glean Magic</t>
+  </si>
+  <si>
+    <t>Divination</t>
+  </si>
+  <si>
+    <t>Inflict Rot</t>
+  </si>
+  <si>
+    <t>Necromancy</t>
+  </si>
+  <si>
+    <t>Miasma of Pestilence</t>
+  </si>
+  <si>
+    <t>Conjuration</t>
+  </si>
+  <si>
+    <t>Overdrive</t>
+  </si>
+  <si>
+    <t>Puddle of Ooze</t>
+  </si>
+  <si>
+    <t>Slicing Shards</t>
+  </si>
+  <si>
+    <t>Static Field</t>
+  </si>
+  <si>
+    <t>Stream of Corruption</t>
+  </si>
+  <si>
+    <t>Acid Arrow</t>
+  </si>
+  <si>
+    <t>Revised</t>
+  </si>
+  <si>
+    <t>Elemental Weapon</t>
+  </si>
+  <si>
+    <t>Flame Arrows</t>
+  </si>
+  <si>
+    <t>Flame Blade</t>
+  </si>
+  <si>
+    <t>Snilloc's Snowball Storm</t>
+  </si>
+  <si>
+    <t>Storm of Vengeance</t>
+  </si>
+  <si>
+    <t>Witch Bolt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,6 +1045,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -944,7 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -968,6 +1099,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="12" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1251,11 +1394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,6 +3152,66 @@
         <v>131</v>
       </c>
       <c r="F85" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B86" s="7">
+        <v>3</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B87" s="7">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B88" s="7">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3087,6 +3290,9 @@
     <hyperlink ref="D82" r:id="rId71" xr:uid="{9EACEB53-922E-4BE1-9434-4CA25F45F00A}"/>
     <hyperlink ref="D83:D84" r:id="rId72" display="A Wicked Brew" xr:uid="{8CC7516F-2F79-47F4-954B-DD7D68021827}"/>
     <hyperlink ref="D85" r:id="rId73" xr:uid="{DA59FB52-321A-4018-A2EA-F3850051FF44}"/>
+    <hyperlink ref="D86" r:id="rId74" xr:uid="{30888777-3C22-4812-8CF7-6C3657A8345E}"/>
+    <hyperlink ref="D87" r:id="rId75" xr:uid="{5BBE3482-35FC-4EA0-AA26-64236FE929AA}"/>
+    <hyperlink ref="D88" r:id="rId76" xr:uid="{693047A9-B752-496F-8718-465CAC53BA65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3094,11 +3300,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,7 +4497,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>131</v>
@@ -4311,7 +4517,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>131</v>
@@ -4331,7 +4537,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>131</v>
@@ -4351,7 +4557,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>131</v>
@@ -4406,6 +4612,26 @@
         <v>36</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4475,9 +4701,10 @@
     <hyperlink ref="A62" r:id="rId61" xr:uid="{D76022EE-A7CB-4E71-9E8F-38BBF0A2D1C0}"/>
     <hyperlink ref="A63" r:id="rId62" xr:uid="{934BAAED-90F7-4112-AC56-DBC1B05CCB8E}"/>
     <hyperlink ref="A64" r:id="rId63" display="Spell Casting Feats" xr:uid="{7866684D-7A4E-4DF6-910F-623213CA2205}"/>
+    <hyperlink ref="A65" r:id="rId64" xr:uid="{C262916F-172D-438D-929F-FED0C5C87A1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId64"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId65"/>
 </worksheet>
 </file>
 
@@ -4486,7 +4713,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4494,37 +4721,37 @@
     <col min="1" max="1" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4945,33 +5172,34 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5002,77 +5230,980 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="9" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C22" s="2">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -5084,50 +6215,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5136,13 +6268,13 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>27</v>
@@ -5162,10 +6294,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>49</v>
@@ -5185,10 +6317,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>27</v>
@@ -5205,13 +6337,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>49</v>
@@ -5257,7 +6389,7 @@
         <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>232</v>
@@ -5358,7 +6490,7 @@
         <v>239</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C11" s="1">
         <v>50000</v>
@@ -5384,7 +6516,7 @@
         <v>242</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="1">
         <v>12000</v>
@@ -5410,7 +6542,7 @@
         <v>243</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>230</v>
@@ -5433,7 +6565,7 @@
         <v>244</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C14" s="1">
         <v>6000</v>
@@ -5485,7 +6617,7 @@
         <v>247</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C16" s="1">
         <v>26000</v>
@@ -5511,7 +6643,7 @@
         <v>248</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C17" s="1">
         <v>7000</v>
@@ -5537,7 +6669,7 @@
         <v>249</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>232</v>
@@ -5583,10 +6715,10 @@
         <v>252</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>27</v>
@@ -5606,7 +6738,7 @@
         <v>253</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>232</v>
@@ -5629,7 +6761,7 @@
         <v>254</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>230</v>
@@ -5652,7 +6784,7 @@
         <v>255</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C23" s="1">
         <v>9000</v>
@@ -5678,7 +6810,7 @@
         <v>256</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>240</v>
@@ -5756,7 +6888,7 @@
         <v>1000</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>49</v>
@@ -5776,7 +6908,7 @@
         <v>263</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C28" s="1">
         <v>3000</v>
@@ -5854,7 +6986,7 @@
         <v>267</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C31" s="1">
         <v>8000</v>
@@ -5932,80 +7064,193 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="Spell Casting Feats" xr:uid="{8D818956-9C64-44E1-881B-897C5E1F6D0F}"/>
+    <hyperlink ref="C3:C6" r:id="rId2" display="Spell Casting Feats" xr:uid="{BD4E7D68-9FA8-40F6-80E5-E0CF18A471B1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{274177BB-5649-4EFE-97E3-7A27204D194E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6015,30 +7260,31 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6084,33 +7330,34 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Public release for monstrous rats
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E61427-42FD-4E62-BF0F-14C899F726F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BA1189-919F-4DA9-859F-010C9D891B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Subclasses!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="334">
   <si>
     <t>Name</t>
   </si>
@@ -1056,6 +1055,30 @@
   </si>
   <si>
     <t>Lore of Vermin</t>
+  </si>
+  <si>
+    <t>Brood Horror</t>
+  </si>
+  <si>
+    <t>Hell Pit Abomination</t>
+  </si>
+  <si>
+    <t>Rat Ogre</t>
+  </si>
+  <si>
+    <t>Wererat</t>
+  </si>
+  <si>
+    <t>Wererat Plague Locus</t>
+  </si>
+  <si>
+    <t>Wolf Rat</t>
+  </si>
+  <si>
+    <t>Rat Monstrosities</t>
+  </si>
+  <si>
+    <t>Hell Pit Abomination should have name change</t>
   </si>
 </sst>
 </file>
@@ -1182,160 +1205,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="114">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="96">
     <dxf>
       <fill>
         <patternFill>
@@ -2428,11 +2298,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,7 +3959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>190</v>
       </c>
@@ -4109,7 +3979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>193</v>
       </c>
@@ -4129,7 +3999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>194</v>
       </c>
@@ -4149,7 +4019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>195</v>
       </c>
@@ -4169,7 +4039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>197</v>
       </c>
@@ -4189,7 +4059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>265</v>
       </c>
@@ -4209,7 +4079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>266</v>
       </c>
@@ -4229,7 +4099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>267</v>
       </c>
@@ -4249,7 +4119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>309</v>
       </c>
@@ -4269,7 +4139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>310</v>
       </c>
@@ -4289,7 +4159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>311</v>
       </c>
@@ -4309,7 +4179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>312</v>
       </c>
@@ -4329,7 +4199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>313</v>
       </c>
@@ -4349,7 +4219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>314</v>
       </c>
@@ -4366,28 +4236,151 @@
         <v>15</v>
       </c>
       <c r="F94" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B95" s="7">
+        <v>10</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B96" s="7">
+        <v>16</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B97" s="7">
+        <v>3</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B98" s="7">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B99" s="7">
+        <v>7</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B100" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4470,19 +4463,21 @@
     <hyperlink ref="D88" r:id="rId76" xr:uid="{693047A9-B752-496F-8718-465CAC53BA65}"/>
     <hyperlink ref="D89" r:id="rId77" xr:uid="{EA81FD11-3461-41B1-B006-E69F57550A4D}"/>
     <hyperlink ref="D90:D94" r:id="rId78" display="Rats" xr:uid="{79B6CD7B-C87E-4410-816A-A16E47DEA79A}"/>
+    <hyperlink ref="D95" r:id="rId79" xr:uid="{A054A175-4D56-424B-A5EE-CE8CD37CE674}"/>
+    <hyperlink ref="D96:D100" r:id="rId80" display="Rat Monstrosities" xr:uid="{B12095CB-C3DA-4859-9EA0-8B69C3713540}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId79"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId81"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5603,7 +5598,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>264</v>
       </c>
@@ -5620,7 +5615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>308</v>
       </c>
@@ -5637,7 +5632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>315</v>
       </c>
@@ -5654,7 +5649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>319</v>
       </c>
@@ -5671,7 +5666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>325</v>
       </c>
@@ -5686,108 +5681,128 @@
       </c>
       <c r="E69" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B24 B33 B40:B1048576">
-    <cfRule type="containsText" dxfId="65" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="59" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="53" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="47" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5860,9 +5875,10 @@
     <hyperlink ref="A67" r:id="rId66" xr:uid="{A5E59BB7-6B0C-4292-BC62-11240AA439EC}"/>
     <hyperlink ref="A68" r:id="rId67" xr:uid="{9529DD90-02A3-453B-87D8-9715CEEDF28B}"/>
     <hyperlink ref="A69" r:id="rId68" xr:uid="{7217EF99-1651-4840-8525-D36C44643DFD}"/>
+    <hyperlink ref="A70" r:id="rId69" xr:uid="{D3FA5FEE-2DA5-49B7-906F-36E776202F93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId69"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId70"/>
 </worksheet>
 </file>
 
@@ -6332,22 +6348,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6429,22 +6445,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7749,42 +7765,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8640,22 +8656,22 @@
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8788,22 +8804,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8887,42 +8903,42 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1:C2 C4:C1048576">
-    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9012,22 +9028,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9113,22 +9129,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add sahuagin to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C02136-2CDB-409C-ADC0-DE4951878E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8CC4EB-B291-4BE5-872A-49296E9F3870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="394">
   <si>
     <t>Name</t>
   </si>
@@ -1254,6 +1254,12 @@
   </si>
   <si>
     <t>New Artificer Infusions</t>
+  </si>
+  <si>
+    <t>Sahuagin</t>
+  </si>
+  <si>
+    <t>Player Race: Sahuagin</t>
   </si>
 </sst>
 </file>
@@ -2578,7 +2584,7 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
@@ -5034,11 +5040,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6359,6 +6365,23 @@
       </c>
       <c r="F75" s="1" t="s">
         <v>347</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6539,9 +6562,10 @@
     <hyperlink ref="A73" r:id="rId72" display="Plague Censer Bearer" xr:uid="{4370DB5D-3FC3-4EB9-A488-FFE7B09B3525}"/>
     <hyperlink ref="A74" r:id="rId73" xr:uid="{C64D2F64-A496-4B75-B25B-8FEC6498C00A}"/>
     <hyperlink ref="A75" r:id="rId74" xr:uid="{4BE50A41-A3BF-44C3-AD1B-B0E6194B9FDA}"/>
+    <hyperlink ref="A76" r:id="rId75" xr:uid="{5BF086D4-5974-483E-9DFB-D1B941F8314B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId75"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId76"/>
 </worksheet>
 </file>
 
@@ -7006,7 +7030,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10341,19 +10365,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
@@ -10401,6 +10425,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C4:C1048576">
@@ -10466,6 +10504,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{274177BB-5649-4EFE-97E3-7A27204D194E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{1A331A7C-2FF4-428B-ABDA-855A9E15AA69}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A96BF5A7-5FA7-4848-8CAA-49C4274F3771}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add all subclasses to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A01504-AB39-43C5-A81F-3D07FB57C271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D005EA1F-200C-4428-9698-4BBA7D13011B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2579" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="530">
   <si>
     <t>Name</t>
   </si>
@@ -1620,6 +1620,54 @@
   </si>
   <si>
     <t>Bard College - College of the Ancients</t>
+  </si>
+  <si>
+    <t>College of Revelry</t>
+  </si>
+  <si>
+    <t>Bard College - College of Revely</t>
+  </si>
+  <si>
+    <t>College of Pacts</t>
+  </si>
+  <si>
+    <t>Bard College - College of Pacts</t>
+  </si>
+  <si>
+    <t>College of Choir</t>
+  </si>
+  <si>
+    <t>College of Finality</t>
+  </si>
+  <si>
+    <t>Bard College - College of Finality</t>
+  </si>
+  <si>
+    <t>Bard College - College of Choir</t>
+  </si>
+  <si>
+    <t>Divine Domain - War</t>
+  </si>
+  <si>
+    <t>Demon Soul</t>
+  </si>
+  <si>
+    <t>Warcaller</t>
+  </si>
+  <si>
+    <t>Path of the Demon Soul</t>
+  </si>
+  <si>
+    <t>Path of the Warcaller</t>
+  </si>
+  <si>
+    <t>Content Dependant</t>
+  </si>
+  <si>
+    <t>Storm Herald</t>
+  </si>
+  <si>
+    <t>Path of the Storm Herald</t>
   </si>
 </sst>
 </file>
@@ -6931,11 +6979,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8768,6 +8816,214 @@
         <v>44</v>
       </c>
       <c r="H70" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H78" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -8863,6 +9119,14 @@
     <hyperlink ref="D68" r:id="rId67" xr:uid="{C8966E9D-D761-4375-875F-F6E20629A00B}"/>
     <hyperlink ref="D69" r:id="rId68" xr:uid="{98D2E4B5-FBB8-431D-8D45-633C093DF6BE}"/>
     <hyperlink ref="D70" r:id="rId69" xr:uid="{9871195F-395C-478C-83EB-B72E72D9F90F}"/>
+    <hyperlink ref="D71" r:id="rId70" xr:uid="{569ED6F0-6807-44B1-85B3-11B58B0EBBD2}"/>
+    <hyperlink ref="D72" r:id="rId71" xr:uid="{B98B347B-FA09-4B42-99F6-7BD49CED4E92}"/>
+    <hyperlink ref="D73" r:id="rId72" display="Bard College - Collge of Choir" xr:uid="{255ABBE8-2EFB-45F1-97D8-C425715B2A80}"/>
+    <hyperlink ref="D74" r:id="rId73" xr:uid="{F2EED849-52B7-47FB-A0A1-7A17556C13E4}"/>
+    <hyperlink ref="D75" r:id="rId74" xr:uid="{55094E7F-6584-49E8-BC8D-A97B7FAA1538}"/>
+    <hyperlink ref="D76" r:id="rId75" display="Primal Path - Demon Soul" xr:uid="{BBF1122C-B61C-4BB5-A8A9-B2CF65AE04FE}"/>
+    <hyperlink ref="D77" r:id="rId76" xr:uid="{D034A541-2381-4E07-AE03-618E15137103}"/>
+    <hyperlink ref="D78" r:id="rId77" xr:uid="{94CA75DD-6633-4D4F-94B4-CECD351EE741}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12217,17 +12481,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -12601,6 +12865,29 @@
         <v>35</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -12634,6 +12921,7 @@
     <hyperlink ref="E14" r:id="rId5" xr:uid="{F16E9818-6A18-4211-B6B9-384E9F193F7C}"/>
     <hyperlink ref="E15" r:id="rId6" xr:uid="{12CCD9A8-AFA3-4FEC-B0C8-CDDB45B44199}"/>
     <hyperlink ref="E16" r:id="rId7" xr:uid="{A8D65C73-7EAB-46C3-90B4-119F84105AE4}"/>
+    <hyperlink ref="E17" r:id="rId8" xr:uid="{2407A640-B6F5-4984-91E5-872F7851A9C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add non-public revised spells to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D005EA1F-200C-4428-9698-4BBA7D13011B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CD368F-CB87-4262-8727-7C0D8E24C8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="544">
   <si>
     <t>Name</t>
   </si>
@@ -1668,6 +1668,48 @@
   </si>
   <si>
     <t>Path of the Storm Herald</t>
+  </si>
+  <si>
+    <t>Revised Spells</t>
+  </si>
+  <si>
+    <t>New Spells</t>
+  </si>
+  <si>
+    <t>Barkskin</t>
+  </si>
+  <si>
+    <t>Compelled Duel</t>
+  </si>
+  <si>
+    <t>Enchantment</t>
+  </si>
+  <si>
+    <t>Crown of Madness</t>
+  </si>
+  <si>
+    <t>Find Hazards</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>Grasping Vine</t>
+  </si>
+  <si>
+    <t>Ray of Enfeeblement</t>
+  </si>
+  <si>
+    <t>Ray of Sickness</t>
+  </si>
+  <si>
+    <t>True Strike</t>
+  </si>
+  <si>
+    <t>Weird</t>
+  </si>
+  <si>
+    <t>Illusion</t>
   </si>
 </sst>
 </file>
@@ -1742,7 +1784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1788,6 +1830,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5451,8 +5499,8 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6561,7 +6609,7 @@
         <v>209</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>44</v>
@@ -6981,7 +7029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
@@ -9137,8 +9185,8 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10138,16 +10186,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
@@ -10162,10 +10210,12 @@
     <col min="13" max="13" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" style="1" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" style="15" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="16" max="16" width="8" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -10211,8 +10261,14 @@
       <c r="O1" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>266</v>
       </c>
@@ -10252,8 +10308,14 @@
       <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>269</v>
       </c>
@@ -10293,8 +10355,14 @@
       <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>270</v>
       </c>
@@ -10334,8 +10402,14 @@
       <c r="M4" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>272</v>
       </c>
@@ -10375,8 +10449,14 @@
       <c r="M5" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>273</v>
       </c>
@@ -10416,8 +10496,14 @@
       <c r="M6" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>206</v>
       </c>
@@ -10457,8 +10543,14 @@
       <c r="M7" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>274</v>
       </c>
@@ -10498,8 +10590,14 @@
       <c r="M8" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>275</v>
       </c>
@@ -10539,8 +10637,14 @@
       <c r="M9" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>277</v>
       </c>
@@ -10580,8 +10684,14 @@
       <c r="M10" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>279</v>
       </c>
@@ -10628,7 +10738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>281</v>
       </c>
@@ -10675,7 +10785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>282</v>
       </c>
@@ -10722,7 +10832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>283</v>
       </c>
@@ -10769,7 +10879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>284</v>
       </c>
@@ -10816,7 +10926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>285</v>
       </c>
@@ -11425,6 +11535,476 @@
       </c>
       <c r="O28" s="15" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O30" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C38" s="2">
+        <v>9</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -11469,6 +12049,10 @@
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="P1" r:id="rId1" xr:uid="{FAD5800B-432F-4DCB-9044-7DD4D8244A6C}"/>
+    <hyperlink ref="Q1" r:id="rId2" xr:uid="{CCBE817D-14F9-4B8B-9826-DAED274C9422}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12485,7 +13069,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12540,7 +13124,7 @@
         <v>326</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -12563,7 +13147,7 @@
         <v>326</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
@@ -12586,7 +13170,7 @@
         <v>326</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>17</v>
@@ -12609,7 +13193,7 @@
         <v>326</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>17</v>
@@ -12632,7 +13216,7 @@
         <v>326</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Clean up non-public new spells
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CD368F-CB87-4262-8727-7C0D8E24C8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C41D1AD-7C50-4D16-8492-30D130652FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="553">
   <si>
     <t>Name</t>
   </si>
@@ -1710,6 +1710,33 @@
   </si>
   <si>
     <t>Illusion</t>
+  </si>
+  <si>
+    <t>Binding Chain</t>
+  </si>
+  <si>
+    <t>Molten Sphere</t>
+  </si>
+  <si>
+    <t>Mud Ball</t>
+  </si>
+  <si>
+    <t>Tranquility</t>
+  </si>
+  <si>
+    <t>Frozen Tomb</t>
+  </si>
+  <si>
+    <t>Water Whip</t>
+  </si>
+  <si>
+    <t>Grasping Tide</t>
+  </si>
+  <si>
+    <t>Stream of Flames</t>
+  </si>
+  <si>
+    <t>Leap Slam</t>
   </si>
 </sst>
 </file>
@@ -7029,8 +7056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
@@ -10186,11 +10213,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12004,6 +12031,429 @@
         <v>35</v>
       </c>
       <c r="O38" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="2">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O41" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O42" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O43" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C46" s="2">
+        <v>6</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O46" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O47" s="15" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean up madness spells and add them to spell list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C41D1AD-7C50-4D16-8492-30D130652FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C29C53-4AB3-4EDB-9B91-58E9FC538BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="557">
   <si>
     <t>Name</t>
   </si>
@@ -1737,6 +1737,18 @@
   </si>
   <si>
     <t>Leap Slam</t>
+  </si>
+  <si>
+    <t>Creeping Smite</t>
+  </si>
+  <si>
+    <t>Fiery Temper</t>
+  </si>
+  <si>
+    <t>Senseless Rage</t>
+  </si>
+  <si>
+    <t>Madness Spells</t>
   </si>
 </sst>
 </file>
@@ -7056,8 +7068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
@@ -10213,11 +10225,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12454,6 +12466,147 @@
         <v>35</v>
       </c>
       <c r="O47" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O48" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O50" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -14110,11 +14263,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D4"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14180,6 +14333,20 @@
         <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -14209,6 +14376,7 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{BD2521FD-FF87-4C8B-99BE-7B21AA39FFD0}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{D4EA4825-1487-4570-B412-DF8E221C1BA1}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{69A08EF4-ECA9-4141-8D49-5C1F1C1827E4}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{7BFC501A-AD63-47FD-B8B6-597E83DED8A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update non-public magic items and add them to content sheet
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C29C53-4AB3-4EDB-9B91-58E9FC538BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD479FC8-532B-41C2-8911-6E29E748BD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">DMResources!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Documents!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Feats!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MagicItems!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MagicItems!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewClassFeatures!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Races!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Spells!$A$1:$O$1</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="602">
   <si>
     <t>Name</t>
   </si>
@@ -1749,6 +1749,141 @@
   </si>
   <si>
     <t>Madness Spells</t>
+  </si>
+  <si>
+    <t>Bank of Abundance</t>
+  </si>
+  <si>
+    <t>New Magic Items</t>
+  </si>
+  <si>
+    <t>Blade of Insight</t>
+  </si>
+  <si>
+    <t>Bracers of the Last Stand</t>
+  </si>
+  <si>
+    <t>Cloak of Daggers</t>
+  </si>
+  <si>
+    <t>Club of Savagery</t>
+  </si>
+  <si>
+    <t>Weapon(Club)</t>
+  </si>
+  <si>
+    <t>Dualist's Standard</t>
+  </si>
+  <si>
+    <t>Enchanted Artisan's Tools</t>
+  </si>
+  <si>
+    <t>Echanted Carriage</t>
+  </si>
+  <si>
+    <t>Ghostfire Blade</t>
+  </si>
+  <si>
+    <t>Weapon (scimitar)</t>
+  </si>
+  <si>
+    <t>Glass Casket</t>
+  </si>
+  <si>
+    <t>Healing Salve</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Jousting Lance</t>
+  </si>
+  <si>
+    <t>Weapon (lance)</t>
+  </si>
+  <si>
+    <t>Light of Restoration</t>
+  </si>
+  <si>
+    <t>Consumable?</t>
+  </si>
+  <si>
+    <t>Mace of the Valiant</t>
+  </si>
+  <si>
+    <t>Weapon (mace)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mantle of Tides </t>
+  </si>
+  <si>
+    <t>Necklace of Xorn</t>
+  </si>
+  <si>
+    <t>Nullifying Chains</t>
+  </si>
+  <si>
+    <t>Orb of Awarness</t>
+  </si>
+  <si>
+    <t>Riot Gear</t>
+  </si>
+  <si>
+    <t>Armor (light, medium, or heavy)</t>
+  </si>
+  <si>
+    <t>Rosethorn Pike</t>
+  </si>
+  <si>
+    <t>Weapon (pike)</t>
+  </si>
+  <si>
+    <t>Rubblemaker</t>
+  </si>
+  <si>
+    <t>Weapon (maul)</t>
+  </si>
+  <si>
+    <t>Rune of Talent</t>
+  </si>
+  <si>
+    <t>Shining Armor</t>
+  </si>
+  <si>
+    <t>Armor (medium or heavy armor made from metal)</t>
+  </si>
+  <si>
+    <t>Smoldering Garrote</t>
+  </si>
+  <si>
+    <t>Weapon (garrote)</t>
+  </si>
+  <si>
+    <t>Spell Bow</t>
+  </si>
+  <si>
+    <t>Weapon (any bow or crossbow)</t>
+  </si>
+  <si>
+    <t>Spore Slinger</t>
+  </si>
+  <si>
+    <t>Weapon (sling)</t>
+  </si>
+  <si>
+    <t>Stalkers Lens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storm Trident </t>
+  </si>
+  <si>
+    <t>Weapon (trident)</t>
+  </si>
+  <si>
+    <t>Wind Cord</t>
+  </si>
+  <si>
+    <t>Whispersilk Cloak</t>
   </si>
 </sst>
 </file>
@@ -12796,28 +12931,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="46.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -12825,844 +12962,1756 @@
         <v>200</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
         <v>100</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
         <v>6000</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1">
         <v>2000</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>15</v>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
         <v>1500</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>219</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
         <v>9000</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
         <v>50000</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
         <v>12000</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>225</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>15</v>
+      <c r="G13" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1">
         <v>6000</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1">
         <v>24000</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1">
         <v>26000</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
         <v>7000</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>232</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>234</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>15</v>
+      <c r="G20" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>15</v>
+      <c r="G21" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>236</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>15</v>
+      <c r="G22" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>237</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1">
         <v>9000</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>15</v>
+      <c r="G23" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>238</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="1">
         <v>20000</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>15</v>
+      <c r="G25" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>214</v>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>214</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>15</v>
+        <v>214</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1">
         <v>1000</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>245</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1">
         <v>3000</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>15</v>
+      <c r="G28" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>246</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="1">
         <v>15000</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>248</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1">
         <v>26000</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>249</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1">
         <v>8000</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
         <v>24000</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>252</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1">
+        <v>500</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="1">
+        <v>50</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="1">
+        <v>75000</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="1">
+        <v>750</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="1">
+        <v>250</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="1">
+        <v>500</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="1">
+        <v>50</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
-  <conditionalFormatting sqref="H1:H1048576">
+  <autoFilter ref="A1:J1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
-      <formula>NOT(ISERROR(SEARCH("Playtest Ready",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
-      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{11FE0D5E-9786-4A71-9B52-12E2A712C6B4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14265,7 +15314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>

</xml_diff>

<commit_message>
Add brass orb and ruined armor to magic items list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD479FC8-532B-41C2-8911-6E29E748BD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC74D948-D291-4BFA-AA39-53B82DA9E945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3288" uniqueCount="606">
   <si>
     <t>Name</t>
   </si>
@@ -1884,6 +1884,18 @@
   </si>
   <si>
     <t>Whispersilk Cloak</t>
+  </si>
+  <si>
+    <t>Ruined Armor, +1</t>
+  </si>
+  <si>
+    <t>Ruined Armor, +2</t>
+  </si>
+  <si>
+    <t>Ruined Armor, +3</t>
+  </si>
+  <si>
+    <t>Brass Orb</t>
   </si>
 </sst>
 </file>
@@ -3214,8 +3226,8 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,7 +5444,7 @@
         <v>15</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -5673,8 +5685,8 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6968,7 +6980,7 @@
         <v>25</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>33</v>
@@ -6988,7 +7000,7 @@
         <v>25</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>33</v>
@@ -12931,11 +12943,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14685,8 +14697,125 @@
         <v>24</v>
       </c>
     </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="1">
+        <v>750</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" s="1">
+        <v>12000</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D67" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>

</xml_diff>

<commit_message>
Add new weapons list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC74D948-D291-4BFA-AA39-53B82DA9E945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88DC0BC-C5A0-4E5C-8895-3606A9E54C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3288" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3334" uniqueCount="615">
   <si>
     <t>Name</t>
   </si>
@@ -1896,6 +1896,33 @@
   </si>
   <si>
     <t>Brass Orb</t>
+  </si>
+  <si>
+    <t>Garrote</t>
+  </si>
+  <si>
+    <t>Poisoned Wind Globe</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Scythe</t>
+  </si>
+  <si>
+    <t>Spike Fist</t>
+  </si>
+  <si>
+    <t>Things Catcher</t>
+  </si>
+  <si>
+    <t>Poisoned Wind Fumigator</t>
+  </si>
+  <si>
+    <t>Spike Fist Brutalist</t>
+  </si>
+  <si>
+    <t>Things Wrangler</t>
   </si>
 </sst>
 </file>
@@ -12809,15 +12836,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACF069B-924A-40FE-91D9-4FC2DC64FE41}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -12910,8 +12937,93 @@
         <v>24</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D5">
+  <conditionalFormatting sqref="D1:D10">
     <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
@@ -12936,6 +13048,11 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{9CCBC16C-3905-4424-A2E4-F4234E908BD0}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{57EA43A4-C943-4D39-AAA9-E3AA59D7BAD8}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{3AFF4EA2-E191-4D8D-8050-71B5E48C8D50}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{3301ABCD-96C1-40CA-AFA1-90143F6DB747}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{A6919838-D682-4D3C-8607-8E30BD0F6F17}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{AD895AE3-6E19-4041-94EC-630DD531692F}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{1733CB9D-AF17-44A3-8D03-D4913043A778}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{FDEB683E-6CD9-47EB-B05F-BFE28BC1A0DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12945,7 +13062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
     </sheetView>
@@ -14846,16 +14963,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -15253,6 +15370,75 @@
         <v>35</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -15287,6 +15473,8 @@
     <hyperlink ref="E15" r:id="rId6" xr:uid="{12CCD9A8-AFA3-4FEC-B0C8-CDDB45B44199}"/>
     <hyperlink ref="E16" r:id="rId7" xr:uid="{A8D65C73-7EAB-46C3-90B4-119F84105AE4}"/>
     <hyperlink ref="E17" r:id="rId8" xr:uid="{2407A640-B6F5-4984-91E5-872F7851A9C8}"/>
+    <hyperlink ref="E18" r:id="rId9" xr:uid="{52881D91-408D-4D5C-A716-A4D7CDD740EB}"/>
+    <hyperlink ref="E19:E20" r:id="rId10" display="New Weapons" xr:uid="{F5339884-D70F-4CD6-9566-0BF8C6533EEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update status of toads
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311B348B-4A8F-4504-A4DD-76C1AAB848F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7D1F42-D552-4E17-AD43-A55A7D11D545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -3255,9 +3255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I109" sqref="I109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4708,7 +4708,7 @@
         <v>166</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -4728,7 +4728,7 @@
         <v>166</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -4748,7 +4748,7 @@
         <v>166</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -4768,7 +4768,7 @@
         <v>166</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -4788,7 +4788,7 @@
         <v>166</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>17</v>
@@ -4808,7 +4808,7 @@
         <v>166</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>17</v>
@@ -4945,10 +4945,10 @@
         <v>171</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>17</v>
@@ -4965,10 +4965,10 @@
         <v>171</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>17</v>
@@ -4985,10 +4985,10 @@
         <v>185</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>17</v>
@@ -5005,10 +5005,10 @@
         <v>171</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>17</v>
@@ -5500,22 +5500,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5590,23 +5590,24 @@
     <hyperlink ref="D78:D79" r:id="rId68" display="Mishipeshu" xr:uid="{BAF42D5B-FD22-4743-8043-DC2F1941E1D8}"/>
     <hyperlink ref="D81" r:id="rId69" xr:uid="{5805A097-BC9D-4685-86E0-E30134117A8D}"/>
     <hyperlink ref="D80" r:id="rId70" xr:uid="{32007A61-8128-435C-8AA0-543B2ECD8C9F}"/>
-    <hyperlink ref="D82" r:id="rId71" xr:uid="{9EACEB53-922E-4BE1-9434-4CA25F45F00A}"/>
-    <hyperlink ref="D83:D84" r:id="rId72" display="A Wicked Brew" xr:uid="{8CC7516F-2F79-47F4-954B-DD7D68021827}"/>
-    <hyperlink ref="D85" r:id="rId73" xr:uid="{DA59FB52-321A-4018-A2EA-F3850051FF44}"/>
-    <hyperlink ref="D86" r:id="rId74" xr:uid="{30888777-3C22-4812-8CF7-6C3657A8345E}"/>
-    <hyperlink ref="D87" r:id="rId75" xr:uid="{5BBE3482-35FC-4EA0-AA26-64236FE929AA}"/>
-    <hyperlink ref="D88" r:id="rId76" xr:uid="{693047A9-B752-496F-8718-465CAC53BA65}"/>
-    <hyperlink ref="D89" r:id="rId77" xr:uid="{EA81FD11-3461-41B1-B006-E69F57550A4D}"/>
-    <hyperlink ref="D90:D94" r:id="rId78" display="Rats" xr:uid="{79B6CD7B-C87E-4410-816A-A16E47DEA79A}"/>
-    <hyperlink ref="D95" r:id="rId79" xr:uid="{A054A175-4D56-424B-A5EE-CE8CD37CE674}"/>
-    <hyperlink ref="D96:D100" r:id="rId80" display="Rat Monstrosities" xr:uid="{B12095CB-C3DA-4859-9EA0-8B69C3713540}"/>
-    <hyperlink ref="D101" r:id="rId81" xr:uid="{F3624BE0-A487-4238-8F0A-AADCDEC764D3}"/>
-    <hyperlink ref="D102:D107" r:id="rId82" display="Sharks" xr:uid="{E63A5F92-E366-4622-8F1F-35F237D7896E}"/>
-    <hyperlink ref="D108" r:id="rId83" display="Plague Censer Bearer" xr:uid="{2F24DF23-C8F6-4EAB-A71D-3AB23DD2112A}"/>
-    <hyperlink ref="D109" r:id="rId84" xr:uid="{33646707-D6F0-4BEA-9AA9-4542677708BF}"/>
+    <hyperlink ref="D86" r:id="rId71" xr:uid="{30888777-3C22-4812-8CF7-6C3657A8345E}"/>
+    <hyperlink ref="D87" r:id="rId72" xr:uid="{5BBE3482-35FC-4EA0-AA26-64236FE929AA}"/>
+    <hyperlink ref="D88" r:id="rId73" xr:uid="{693047A9-B752-496F-8718-465CAC53BA65}"/>
+    <hyperlink ref="D89" r:id="rId74" xr:uid="{EA81FD11-3461-41B1-B006-E69F57550A4D}"/>
+    <hyperlink ref="D90:D94" r:id="rId75" display="Rats" xr:uid="{79B6CD7B-C87E-4410-816A-A16E47DEA79A}"/>
+    <hyperlink ref="D95" r:id="rId76" xr:uid="{A054A175-4D56-424B-A5EE-CE8CD37CE674}"/>
+    <hyperlink ref="D96:D100" r:id="rId77" display="Rat Monstrosities" xr:uid="{B12095CB-C3DA-4859-9EA0-8B69C3713540}"/>
+    <hyperlink ref="D101" r:id="rId78" xr:uid="{F3624BE0-A487-4238-8F0A-AADCDEC764D3}"/>
+    <hyperlink ref="D102:D107" r:id="rId79" display="Sharks" xr:uid="{E63A5F92-E366-4622-8F1F-35F237D7896E}"/>
+    <hyperlink ref="D108" r:id="rId80" display="Plague Censer Bearer" xr:uid="{2F24DF23-C8F6-4EAB-A71D-3AB23DD2112A}"/>
+    <hyperlink ref="D109" r:id="rId81" xr:uid="{33646707-D6F0-4BEA-9AA9-4542677708BF}"/>
+    <hyperlink ref="D82" r:id="rId82" xr:uid="{EAE0F169-94E4-4969-A7AE-9180BFEAC64F}"/>
+    <hyperlink ref="D83" r:id="rId83" xr:uid="{9B127A72-3026-4FB4-8588-E931E54A6ED2}"/>
+    <hyperlink ref="D84" r:id="rId84" xr:uid="{E0FD2177-4EF5-4418-9EE2-3BFFDCDD721A}"/>
+    <hyperlink ref="D85" r:id="rId85" xr:uid="{B3A78307-9664-44DC-AD02-B96E81A7AE4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId85"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId86"/>
 </worksheet>
 </file>
 
@@ -5683,22 +5684,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5716,7 +5717,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6650,7 +6651,7 @@
         <v>166</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>25</v>
@@ -7090,102 +7091,102 @@
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B24 B33 B40:B1048576">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7275,7 +7276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
@@ -9350,22 +9351,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10396,22 +10397,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12847,42 +12848,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="89" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13084,22 +13085,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14994,22 +14995,22 @@
   <autoFilter ref="A1:J1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15505,22 +15506,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15619,62 +15620,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C4:C1048576">
-    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15779,22 +15780,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Sea Fish Part 1 Public Release
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311B348B-4A8F-4504-A4DD-76C1AAB848F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5DE0A7-E197-461E-A194-C46C6918923B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3342" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3382" uniqueCount="630">
   <si>
     <t>Name</t>
   </si>
@@ -1926,6 +1926,48 @@
   </si>
   <si>
     <t>Otherworldly Patron - The Undead</t>
+  </si>
+  <si>
+    <t>Barracuda</t>
+  </si>
+  <si>
+    <t>Giant Barracuda</t>
+  </si>
+  <si>
+    <t>School of Barracuda</t>
+  </si>
+  <si>
+    <t>Lionfish</t>
+  </si>
+  <si>
+    <t>Giant Lionfish</t>
+  </si>
+  <si>
+    <t>Pufferfish</t>
+  </si>
+  <si>
+    <t>Giant Pufferfish</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 1</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 2</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 3</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 4</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 5</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 6</t>
+  </si>
+  <si>
+    <t>Sea Fish Part 7</t>
   </si>
 </sst>
 </file>
@@ -3253,11 +3295,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I109" sqref="I109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4708,7 +4750,7 @@
         <v>166</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>17</v>
@@ -4728,7 +4770,7 @@
         <v>166</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>17</v>
@@ -4748,7 +4790,7 @@
         <v>166</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -4768,7 +4810,7 @@
         <v>166</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -4788,7 +4830,7 @@
         <v>166</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>17</v>
@@ -4808,7 +4850,7 @@
         <v>166</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>17</v>
@@ -4945,10 +4987,10 @@
         <v>171</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>17</v>
@@ -4965,10 +5007,10 @@
         <v>171</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>17</v>
@@ -4985,10 +5027,10 @@
         <v>185</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>17</v>
@@ -5005,10 +5047,10 @@
         <v>171</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>17</v>
@@ -5497,8 +5539,149 @@
         <v>24</v>
       </c>
     </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B110" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B111" s="7">
+        <v>1</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B112" s="7">
+        <v>3</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B113" s="7">
+        <v>0</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B114" s="7">
+        <v>3</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B115" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B116" s="7">
+        <v>4</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
@@ -5590,23 +5773,26 @@
     <hyperlink ref="D78:D79" r:id="rId68" display="Mishipeshu" xr:uid="{BAF42D5B-FD22-4743-8043-DC2F1941E1D8}"/>
     <hyperlink ref="D81" r:id="rId69" xr:uid="{5805A097-BC9D-4685-86E0-E30134117A8D}"/>
     <hyperlink ref="D80" r:id="rId70" xr:uid="{32007A61-8128-435C-8AA0-543B2ECD8C9F}"/>
-    <hyperlink ref="D82" r:id="rId71" xr:uid="{9EACEB53-922E-4BE1-9434-4CA25F45F00A}"/>
-    <hyperlink ref="D83:D84" r:id="rId72" display="A Wicked Brew" xr:uid="{8CC7516F-2F79-47F4-954B-DD7D68021827}"/>
-    <hyperlink ref="D85" r:id="rId73" xr:uid="{DA59FB52-321A-4018-A2EA-F3850051FF44}"/>
-    <hyperlink ref="D86" r:id="rId74" xr:uid="{30888777-3C22-4812-8CF7-6C3657A8345E}"/>
-    <hyperlink ref="D87" r:id="rId75" xr:uid="{5BBE3482-35FC-4EA0-AA26-64236FE929AA}"/>
-    <hyperlink ref="D88" r:id="rId76" xr:uid="{693047A9-B752-496F-8718-465CAC53BA65}"/>
-    <hyperlink ref="D89" r:id="rId77" xr:uid="{EA81FD11-3461-41B1-B006-E69F57550A4D}"/>
-    <hyperlink ref="D90:D94" r:id="rId78" display="Rats" xr:uid="{79B6CD7B-C87E-4410-816A-A16E47DEA79A}"/>
-    <hyperlink ref="D95" r:id="rId79" xr:uid="{A054A175-4D56-424B-A5EE-CE8CD37CE674}"/>
-    <hyperlink ref="D96:D100" r:id="rId80" display="Rat Monstrosities" xr:uid="{B12095CB-C3DA-4859-9EA0-8B69C3713540}"/>
-    <hyperlink ref="D101" r:id="rId81" xr:uid="{F3624BE0-A487-4238-8F0A-AADCDEC764D3}"/>
-    <hyperlink ref="D102:D107" r:id="rId82" display="Sharks" xr:uid="{E63A5F92-E366-4622-8F1F-35F237D7896E}"/>
-    <hyperlink ref="D108" r:id="rId83" display="Plague Censer Bearer" xr:uid="{2F24DF23-C8F6-4EAB-A71D-3AB23DD2112A}"/>
-    <hyperlink ref="D109" r:id="rId84" xr:uid="{33646707-D6F0-4BEA-9AA9-4542677708BF}"/>
+    <hyperlink ref="D86" r:id="rId71" xr:uid="{30888777-3C22-4812-8CF7-6C3657A8345E}"/>
+    <hyperlink ref="D87" r:id="rId72" xr:uid="{5BBE3482-35FC-4EA0-AA26-64236FE929AA}"/>
+    <hyperlink ref="D88" r:id="rId73" xr:uid="{693047A9-B752-496F-8718-465CAC53BA65}"/>
+    <hyperlink ref="D89" r:id="rId74" xr:uid="{EA81FD11-3461-41B1-B006-E69F57550A4D}"/>
+    <hyperlink ref="D90:D94" r:id="rId75" display="Rats" xr:uid="{79B6CD7B-C87E-4410-816A-A16E47DEA79A}"/>
+    <hyperlink ref="D95" r:id="rId76" xr:uid="{A054A175-4D56-424B-A5EE-CE8CD37CE674}"/>
+    <hyperlink ref="D96:D100" r:id="rId77" display="Rat Monstrosities" xr:uid="{B12095CB-C3DA-4859-9EA0-8B69C3713540}"/>
+    <hyperlink ref="D101" r:id="rId78" xr:uid="{F3624BE0-A487-4238-8F0A-AADCDEC764D3}"/>
+    <hyperlink ref="D102:D107" r:id="rId79" display="Sharks" xr:uid="{E63A5F92-E366-4622-8F1F-35F237D7896E}"/>
+    <hyperlink ref="D108" r:id="rId80" display="Plague Censer Bearer" xr:uid="{2F24DF23-C8F6-4EAB-A71D-3AB23DD2112A}"/>
+    <hyperlink ref="D109" r:id="rId81" xr:uid="{33646707-D6F0-4BEA-9AA9-4542677708BF}"/>
+    <hyperlink ref="D82" r:id="rId82" xr:uid="{EAE0F169-94E4-4969-A7AE-9180BFEAC64F}"/>
+    <hyperlink ref="D83" r:id="rId83" xr:uid="{9B127A72-3026-4FB4-8588-E931E54A6ED2}"/>
+    <hyperlink ref="D84" r:id="rId84" xr:uid="{E0FD2177-4EF5-4418-9EE2-3BFFDCDD721A}"/>
+    <hyperlink ref="D85" r:id="rId85" xr:uid="{B3A78307-9664-44DC-AD02-B96E81A7AE4A}"/>
+    <hyperlink ref="D110" r:id="rId86" xr:uid="{146F3E03-09A2-4512-BB9A-2C060513EEC9}"/>
+    <hyperlink ref="D111:D116" r:id="rId87" display="Sea Fish Part 1" xr:uid="{145A0FED-0D36-4059-A3D2-CCBD8704EAF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId85"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId88"/>
 </worksheet>
 </file>
 
@@ -5712,11 +5898,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6650,7 +6836,7 @@
         <v>166</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>25</v>
@@ -7083,6 +7269,23 @@
         <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7265,9 +7468,10 @@
     <hyperlink ref="A74" r:id="rId73" xr:uid="{C64D2F64-A496-4B75-B25B-8FEC6498C00A}"/>
     <hyperlink ref="A75" r:id="rId74" xr:uid="{4BE50A41-A3BF-44C3-AD1B-B0E6194B9FDA}"/>
     <hyperlink ref="A76" r:id="rId75" xr:uid="{5BF086D4-5974-483E-9DFB-D1B941F8314B}"/>
+    <hyperlink ref="A77" r:id="rId76" xr:uid="{FEA4C503-4FF2-4C28-8A10-9EF08B948C47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId76"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId77"/>
 </worksheet>
 </file>
 
@@ -7275,7 +7479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
@@ -12899,7 +13103,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add goose ribbon and update goose content status
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53331CB2-2134-4067-AC39-F114FF5AB5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D0E35A-6E02-428C-B6E0-ED65942F829A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3394" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="627">
   <si>
     <t>Name</t>
   </si>
@@ -1956,6 +1956,9 @@
   </si>
   <si>
     <t>Packmasters</t>
+  </si>
+  <si>
+    <t>Goose Ribbon</t>
   </si>
 </sst>
 </file>
@@ -3286,8 +3289,8 @@
   <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E118" sqref="E118"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4498,7 +4501,7 @@
         <v>149</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>17</v>
@@ -4518,7 +4521,7 @@
         <v>149</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>17</v>
@@ -4538,7 +4541,7 @@
         <v>149</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>17</v>
@@ -4558,7 +4561,7 @@
         <v>149</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>17</v>
@@ -4578,7 +4581,7 @@
         <v>149</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>17</v>
@@ -5894,8 +5897,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6749,10 +6752,10 @@
         <v>149</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>17</v>
@@ -6832,7 +6835,7 @@
         <v>57</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>17</v>
@@ -6966,7 +6969,7 @@
         <v>57</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>17</v>
@@ -6983,7 +6986,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>17</v>
@@ -7000,7 +7003,7 @@
         <v>57</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>17</v>
@@ -13359,11 +13362,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15227,6 +15230,32 @@
       </c>
       <c r="J67" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Maiden of the Mountain to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF7A833-974E-431C-B851-EA298E9D3C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A18DCE-E070-4951-877C-0DAA70158FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3407" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="631">
   <si>
     <t>Name</t>
   </si>
@@ -1962,6 +1962,15 @@
   </si>
   <si>
     <t>Packmaster</t>
+  </si>
+  <si>
+    <t>Maiden of the Mouantain</t>
+  </si>
+  <si>
+    <t>Maiden of the Mountain</t>
+  </si>
+  <si>
+    <t>0.0.0</t>
   </si>
 </sst>
 </file>
@@ -2094,7 +2103,109 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="114">
+  <dxfs count="126">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5748,42 +5859,42 @@
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E1:E108 E110:E1048576">
-    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="125" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="124" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="123" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="122" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="121" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="120" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E109)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5889,17 +6000,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
@@ -5957,31 +6068,49 @@
         <v>34</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="In Development">
+      <formula>NOT(ISERROR(SEARCH("In Development",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3EFAC9F1-5F5A-4C59-93FD-3C2D517B2D1E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{7B705A5F-9E61-4ED2-9B92-55A7CA95D80D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{D8A3A87D-9811-44A2-BC0C-F580D8CAFACE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5991,7 +6120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
@@ -7424,102 +7553,102 @@
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B24 B33 B40:B1048576">
-    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7614,7 +7743,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9687,22 +9816,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="111" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="110" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="108" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10733,22 +10862,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13184,42 +13313,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13421,22 +13550,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15357,22 +15486,22 @@
   <autoFilter ref="A1:J1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15868,22 +15997,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15982,62 +16111,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C4:C1048576">
-    <cfRule type="containsText" dxfId="65" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16142,22 +16271,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add fish to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A18DCE-E070-4951-877C-0DAA70158FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A873D9FD-2CC8-49C3-9109-500796963553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="640">
   <si>
     <t>Name</t>
   </si>
@@ -1971,6 +1971,33 @@
   </si>
   <si>
     <t>0.0.0</t>
+  </si>
+  <si>
+    <t>Giant Anglerfish</t>
+  </si>
+  <si>
+    <t>Largetooth Sawfish</t>
+  </si>
+  <si>
+    <t>Smalltooth Sawfish</t>
+  </si>
+  <si>
+    <t>Giant Stargazer</t>
+  </si>
+  <si>
+    <t>Stonefish</t>
+  </si>
+  <si>
+    <t>Giant Stonefish</t>
+  </si>
+  <si>
+    <t>Swordfish</t>
+  </si>
+  <si>
+    <t>Great Swordfish</t>
+  </si>
+  <si>
+    <t>Sea Fish: Part 2</t>
   </si>
 </sst>
 </file>
@@ -2103,109 +2130,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="114">
     <dxf>
       <fill>
         <patternFill>
@@ -3451,11 +3376,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E118" sqref="E118"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5855,46 +5780,206 @@
         <v>24</v>
       </c>
     </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B118" s="7">
+        <v>7</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B119" s="7">
+        <v>1</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B120" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B121" s="7">
+        <v>6</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B122" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B123" s="7">
+        <v>5</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B124" s="7">
+        <v>1</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B125" s="7">
+        <v>3</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E1:E108 E110:E1048576">
-    <cfRule type="containsText" dxfId="125" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109">
-    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E109)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5992,9 +6077,17 @@
     <hyperlink ref="D115" r:id="rId91" xr:uid="{7CAD7860-0680-42E3-B03B-D18977817009}"/>
     <hyperlink ref="D116" r:id="rId92" xr:uid="{AF80B0BE-98C2-4267-A3D5-EF7DCD1F269A}"/>
     <hyperlink ref="D117" r:id="rId93" xr:uid="{42685035-A275-432B-9D3F-F81DC15AB39E}"/>
+    <hyperlink ref="D118" r:id="rId94" xr:uid="{0086C50D-5303-47F1-B210-19AA231A0499}"/>
+    <hyperlink ref="D119" r:id="rId95" xr:uid="{842EAA2C-8EC8-4566-9E3D-91226725B758}"/>
+    <hyperlink ref="D120" r:id="rId96" xr:uid="{BE8A54D6-3919-4AEA-9CBD-F7A3795D6BBC}"/>
+    <hyperlink ref="D122" r:id="rId97" xr:uid="{E5647353-F310-4E63-94E1-75224878684B}"/>
+    <hyperlink ref="D124" r:id="rId98" xr:uid="{78F7197B-983B-4445-9D18-2525E847904C}"/>
+    <hyperlink ref="D121" r:id="rId99" xr:uid="{0AE1DAFD-5F85-40AF-85AE-9A4B19E50749}"/>
+    <hyperlink ref="D123" r:id="rId100" xr:uid="{1C76907A-21AC-4CA5-B96E-C5C12C3971AB}"/>
+    <hyperlink ref="D125" r:id="rId101" xr:uid="{884ACE17-788C-4EA9-A985-33E2E565411C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId94"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId102"/>
 </worksheet>
 </file>
 
@@ -6002,7 +6095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
@@ -6088,22 +6181,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6118,11 +6211,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7549,106 +7642,123 @@
         <v>345</v>
       </c>
     </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B24 B33 B40:B1048576">
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="35" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7731,9 +7841,10 @@
     <hyperlink ref="A77" r:id="rId76" xr:uid="{73CD645D-EE3A-4108-984E-1F9CE9A98B4C}"/>
     <hyperlink ref="A78" r:id="rId77" xr:uid="{E467B59A-C519-4CE0-81FE-688EB1E176AF}"/>
     <hyperlink ref="A79" r:id="rId78" xr:uid="{8156C637-1110-4572-90DC-540E32C212CA}"/>
+    <hyperlink ref="A80" r:id="rId79" xr:uid="{6E53C99C-B755-4860-A6DC-A38001C6B94F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId79"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId80"/>
 </worksheet>
 </file>
 
@@ -9816,22 +9927,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10862,22 +10973,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10928,8 +11039,8 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13313,42 +13424,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13550,22 +13661,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15486,22 +15597,22 @@
   <autoFilter ref="A1:J1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15997,22 +16108,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16111,62 +16222,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C4:C1048576">
-    <cfRule type="containsText" dxfId="71" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="65" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16271,22 +16382,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update cantrip invocation status
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7654CB7-CF8D-4CC3-891B-C16C32A40ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371313C8-8781-4BEF-A428-E00D529E90A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -6193,9 +6193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7229,7 +7229,7 @@
         <v>187</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>44</v>
@@ -10014,9 +10014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10064,7 +10064,7 @@
         <v>187</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
@@ -10084,7 +10084,7 @@
         <v>187</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
@@ -10104,7 +10104,7 @@
         <v>187</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
@@ -10124,7 +10124,7 @@
         <v>187</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
@@ -10144,7 +10144,7 @@
         <v>187</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
@@ -10164,7 +10164,7 @@
         <v>187</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
@@ -10184,7 +10184,7 @@
         <v>187</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>17</v>
@@ -10204,7 +10204,7 @@
         <v>187</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
@@ -10224,7 +10224,7 @@
         <v>187</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>17</v>
@@ -10244,7 +10244,7 @@
         <v>187</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
@@ -10264,7 +10264,7 @@
         <v>187</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>17</v>
@@ -10284,7 +10284,7 @@
         <v>187</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>17</v>
@@ -10304,7 +10304,7 @@
         <v>187</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>17</v>
@@ -10324,7 +10324,7 @@
         <v>187</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>17</v>
@@ -10344,7 +10344,7 @@
         <v>187</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>17</v>
@@ -10364,7 +10364,7 @@
         <v>187</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
@@ -10384,7 +10384,7 @@
         <v>187</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
@@ -10404,7 +10404,7 @@
         <v>187</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
@@ -10424,7 +10424,7 @@
         <v>187</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>17</v>
@@ -10444,7 +10444,7 @@
         <v>187</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Finish clean up of spell casting feats
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FECE6C-A43A-47E2-98C7-991E7749C5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED968FAE-E83E-423A-8A16-30C60E0FEBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -3327,7 +3327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
@@ -6139,9 +6139,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7006,9 +7006,6 @@
       <c r="E49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F49" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -7086,9 +7083,6 @@
       <c r="E53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="1">
-        <v>5</v>
-      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
@@ -7209,7 +7203,7 @@
         <v>204</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>44</v>
@@ -7226,7 +7220,7 @@
         <v>205</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>44</v>
@@ -7243,7 +7237,7 @@
         <v>206</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>44</v>
@@ -7277,7 +7271,7 @@
         <v>209</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>44</v>
@@ -10965,8 +10959,8 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15556,7 +15550,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15611,7 +15605,7 @@
         <v>326</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -15634,7 +15628,7 @@
         <v>326</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
@@ -15657,7 +15651,7 @@
         <v>326</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>17</v>
@@ -15680,7 +15674,7 @@
         <v>326</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>17</v>
@@ -15703,7 +15697,7 @@
         <v>326</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>17</v>
@@ -16055,15 +16049,13 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{8D818956-9C64-44E1-881B-897C5E1F6D0F}"/>
-    <hyperlink ref="E3:E6" r:id="rId2" display="Independent Feats" xr:uid="{21464BF6-6E4D-4716-87A6-414741373543}"/>
-    <hyperlink ref="E7:E9" r:id="rId3" display="Independent Feats" xr:uid="{9BC31011-BDCB-4ED2-A0CD-AA6B3E0B9EDA}"/>
-    <hyperlink ref="E10:E13" r:id="rId4" display="Independent Feats" xr:uid="{E9F4BC65-574C-491C-B12F-C8754FF27EC4}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{F16E9818-6A18-4211-B6B9-384E9F193F7C}"/>
-    <hyperlink ref="E15" r:id="rId6" xr:uid="{12CCD9A8-AFA3-4FEC-B0C8-CDDB45B44199}"/>
-    <hyperlink ref="E16" r:id="rId7" xr:uid="{A8D65C73-7EAB-46C3-90B4-119F84105AE4}"/>
-    <hyperlink ref="E17" r:id="rId8" xr:uid="{2407A640-B6F5-4984-91E5-872F7851A9C8}"/>
-    <hyperlink ref="E18" r:id="rId9" xr:uid="{52881D91-408D-4D5C-A716-A4D7CDD740EB}"/>
-    <hyperlink ref="E19:E20" r:id="rId10" display="New Weapons" xr:uid="{F5339884-D70F-4CD6-9566-0BF8C6533EEC}"/>
+    <hyperlink ref="E14" r:id="rId2" xr:uid="{F16E9818-6A18-4211-B6B9-384E9F193F7C}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{12CCD9A8-AFA3-4FEC-B0C8-CDDB45B44199}"/>
+    <hyperlink ref="E17" r:id="rId4" xr:uid="{2407A640-B6F5-4984-91E5-872F7851A9C8}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{52881D91-408D-4D5C-A716-A4D7CDD740EB}"/>
+    <hyperlink ref="E19:E20" r:id="rId6" display="New Weapons" xr:uid="{F5339884-D70F-4CD6-9566-0BF8C6533EEC}"/>
+    <hyperlink ref="E3:E13" r:id="rId7" display="Independent Feats" xr:uid="{25EAA3AF-808E-4703-B673-65CF6287924C}"/>
+    <hyperlink ref="E16" r:id="rId8" xr:uid="{9F511F09-57B3-468D-A291-0A53F0941DE3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Isonade to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE77502-0FD8-46F4-B925-3DD46BCFC09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6048F5-A201-4D62-BE26-350A4A0A9645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3467" uniqueCount="641">
   <si>
     <t>Name</t>
   </si>
@@ -1998,6 +1998,9 @@
   </si>
   <si>
     <t>Sea Fish: Part 2</t>
+  </si>
+  <si>
+    <t>Isonade</t>
   </si>
 </sst>
 </file>
@@ -3325,11 +3328,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5886,6 +5889,26 @@
         <v>15</v>
       </c>
       <c r="F125" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B126" s="7">
+        <v>7</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6011,9 +6034,10 @@
     <hyperlink ref="D80" r:id="rId96" xr:uid="{3C34D46C-8B2A-44CC-8679-43078C103696}"/>
     <hyperlink ref="D81" r:id="rId97" xr:uid="{FC60EF05-7038-4200-BC21-E571C114C54C}"/>
     <hyperlink ref="D38:D41" r:id="rId98" display="Otters" xr:uid="{5B129CAF-5388-4616-B378-0AC02F569450}"/>
+    <hyperlink ref="D126" r:id="rId99" xr:uid="{8FD7497B-7CAD-4106-9444-6EDC680D286F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId99"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId100"/>
 </worksheet>
 </file>
 
@@ -6137,11 +6161,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7576,6 +7600,23 @@
         <v>17</v>
       </c>
       <c r="E80" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7762,9 +7803,10 @@
     <hyperlink ref="A79" r:id="rId77" xr:uid="{8156C637-1110-4572-90DC-540E32C212CA}"/>
     <hyperlink ref="A80" r:id="rId78" xr:uid="{6E53C99C-B755-4860-A6DC-A38001C6B94F}"/>
     <hyperlink ref="A27" r:id="rId79" xr:uid="{16E9931D-7C2E-4EF8-BC63-A0EEEE0978EC}"/>
+    <hyperlink ref="A81" r:id="rId80" xr:uid="{D7FFA073-CBFE-4427-B861-B23FB6A1C0F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId80"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId81"/>
 </worksheet>
 </file>
 
@@ -10958,7 +11000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>

</xml_diff>

<commit_message>
Update status of water horse content
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6048F5-A201-4D62-BE26-350A4A0A9645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99E9FA1-9247-47A4-A194-287AEFDBB978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">DMResources!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Documents!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Feats!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MagicItems!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MagicItems!$A$1:$K$69</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewClassFeatures!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Races!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Spells!$A$1:$O$1</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3467" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="642">
   <si>
     <t>Name</t>
   </si>
@@ -2001,6 +2001,9 @@
   </si>
   <si>
     <t>Isonade</t>
+  </si>
+  <si>
+    <t>Cold Iron Tack</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2136,211 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="132">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3330,9 +3537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C136" sqref="C136"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4703,7 +4910,7 @@
         <v>160</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>115</v>
+        <v>294</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>17</v>
@@ -4723,7 +4930,7 @@
         <v>160</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>115</v>
+        <v>294</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>17</v>
@@ -4743,7 +4950,7 @@
         <v>160</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>115</v>
+        <v>294</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>17</v>
@@ -4763,7 +4970,7 @@
         <v>164</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -5915,24 +6122,84 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="E1:E65 E69:E1048576">
+    <cfRule type="containsText" dxfId="131" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="130" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="129" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="128" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="127" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="126" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="containsText" dxfId="125" priority="13" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",E66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="14" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="15" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="122" priority="16" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="17" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="18" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="containsText" dxfId="119" priority="7" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",E67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="8" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="9" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="10" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="11" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="12" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",E68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="4" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="6" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -6131,22 +6398,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6165,7 +6432,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7056,7 +7323,7 @@
         <v>160</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>25</v>
@@ -7076,7 +7343,7 @@
         <v>164</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>25</v>
@@ -7623,104 +7890,124 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B24 B33 B40:B1048576">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="B1:B24 B33 B53:B1048576 B40:B51">
+    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -9889,22 +10176,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10935,22 +11222,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13386,42 +13673,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="89" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13438,7 +13725,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13623,22 +13910,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13659,11 +13946,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13676,9 +13963,9 @@
     <col min="6" max="6" width="21.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -13713,8 +14000,8 @@
       <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>558</v>
+      <c r="K1" s="9" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -13745,6 +14032,9 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -13771,6 +14061,9 @@
       <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -13797,6 +14090,9 @@
       <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -13823,6 +14119,9 @@
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -13852,6 +14151,9 @@
       <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K6" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -13878,6 +14180,9 @@
       <c r="J7" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K7" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -13907,6 +14212,9 @@
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K8" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -13936,6 +14244,9 @@
       <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K9" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -13965,6 +14276,9 @@
       <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K10" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -13994,6 +14308,9 @@
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K11" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -14023,6 +14340,9 @@
       <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K12" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -14049,6 +14369,9 @@
       <c r="J13" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K13" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -14078,6 +14401,9 @@
       <c r="J14" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K14" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -14107,6 +14433,9 @@
       <c r="J15" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K15" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -14136,8 +14465,11 @@
       <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>230</v>
       </c>
@@ -14165,8 +14497,11 @@
       <c r="J17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>231</v>
       </c>
@@ -14191,8 +14526,11 @@
       <c r="J18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>232</v>
       </c>
@@ -14217,8 +14555,11 @@
       <c r="J19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>234</v>
       </c>
@@ -14243,8 +14584,11 @@
       <c r="J20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>235</v>
       </c>
@@ -14269,8 +14613,11 @@
       <c r="J21" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>236</v>
       </c>
@@ -14295,8 +14642,11 @@
       <c r="J22" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>237</v>
       </c>
@@ -14324,8 +14674,11 @@
       <c r="J23" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>238</v>
       </c>
@@ -14350,8 +14703,11 @@
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>239</v>
       </c>
@@ -14379,8 +14735,11 @@
       <c r="J25" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>241</v>
       </c>
@@ -14405,8 +14764,11 @@
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>243</v>
       </c>
@@ -14434,8 +14796,11 @@
       <c r="J27" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>245</v>
       </c>
@@ -14463,8 +14828,11 @@
       <c r="J28" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>246</v>
       </c>
@@ -14492,8 +14860,11 @@
       <c r="J29" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>248</v>
       </c>
@@ -14521,8 +14892,11 @@
       <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>249</v>
       </c>
@@ -14550,8 +14924,11 @@
       <c r="J31" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>250</v>
       </c>
@@ -14579,8 +14956,11 @@
       <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>252</v>
       </c>
@@ -14605,8 +14985,11 @@
       <c r="J33" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>557</v>
       </c>
@@ -14634,8 +15017,11 @@
       <c r="J34" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>559</v>
       </c>
@@ -14660,8 +15046,11 @@
       <c r="J35" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>560</v>
       </c>
@@ -14686,8 +15075,11 @@
       <c r="J36" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>561</v>
       </c>
@@ -14712,8 +15104,11 @@
       <c r="J37" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>562</v>
       </c>
@@ -14738,8 +15133,11 @@
       <c r="J38" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>564</v>
       </c>
@@ -14764,8 +15162,11 @@
       <c r="J39" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>565</v>
       </c>
@@ -14793,8 +15194,11 @@
       <c r="J40" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>566</v>
       </c>
@@ -14822,8 +15226,11 @@
       <c r="J41" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>567</v>
       </c>
@@ -14848,8 +15255,11 @@
       <c r="J42" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>569</v>
       </c>
@@ -14874,8 +15284,11 @@
       <c r="J43" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>570</v>
       </c>
@@ -14903,8 +15316,11 @@
       <c r="J44" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>572</v>
       </c>
@@ -14929,8 +15345,11 @@
       <c r="J45" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>574</v>
       </c>
@@ -14958,8 +15377,11 @@
       <c r="J46" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>576</v>
       </c>
@@ -14984,8 +15406,11 @@
       <c r="J47" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>578</v>
       </c>
@@ -15010,8 +15435,11 @@
       <c r="J48" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>579</v>
       </c>
@@ -15039,8 +15467,11 @@
       <c r="J49" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>580</v>
       </c>
@@ -15068,8 +15499,11 @@
       <c r="J50" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>581</v>
       </c>
@@ -15097,8 +15531,11 @@
       <c r="J51" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>582</v>
       </c>
@@ -15123,8 +15560,11 @@
       <c r="J52" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>584</v>
       </c>
@@ -15149,8 +15589,11 @@
       <c r="J53" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>586</v>
       </c>
@@ -15175,8 +15618,11 @@
       <c r="J54" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>588</v>
       </c>
@@ -15204,8 +15650,11 @@
       <c r="J55" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>589</v>
       </c>
@@ -15230,8 +15679,11 @@
       <c r="J56" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>591</v>
       </c>
@@ -15256,8 +15708,11 @@
       <c r="J57" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>593</v>
       </c>
@@ -15282,8 +15737,11 @@
       <c r="J58" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>595</v>
       </c>
@@ -15308,8 +15766,11 @@
       <c r="J59" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>597</v>
       </c>
@@ -15334,8 +15795,11 @@
       <c r="J60" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>598</v>
       </c>
@@ -15360,8 +15824,11 @@
       <c r="J61" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>600</v>
       </c>
@@ -15386,8 +15853,11 @@
       <c r="J62" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>601</v>
       </c>
@@ -15412,8 +15882,11 @@
       <c r="J63" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>602</v>
       </c>
@@ -15441,8 +15914,11 @@
       <c r="J64" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>603</v>
       </c>
@@ -15470,8 +15946,11 @@
       <c r="J65" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>604</v>
       </c>
@@ -15499,8 +15978,11 @@
       <c r="J66" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>605</v>
       </c>
@@ -15528,8 +16010,11 @@
       <c r="J67" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>626</v>
       </c>
@@ -15554,35 +16039,69 @@
       <c r="J68" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K68" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
+  <autoFilter ref="A1:K69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K1" r:id="rId1" xr:uid="{11FE0D5E-9786-4A71-9B52-12E2A712C6B4}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{7F5C5684-5944-4475-9E96-4CDA45D63C85}"/>
+    <hyperlink ref="K3:K68" r:id="rId2" display="New Magic Items" xr:uid="{0B420A92-4474-4787-B4FF-A1555810215A}"/>
+    <hyperlink ref="K69" r:id="rId3" xr:uid="{1FB46F41-6996-47A9-AE07-5FCDCDB4395E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -16070,22 +16589,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16182,62 +16701,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C5:C1048576">
-    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16342,22 +16861,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update status of beaver content
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99E9FA1-9247-47A4-A194-287AEFDBB978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B577E9-0979-4205-B79A-EC865B6605B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -3539,7 +3539,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+      <selection pane="bottomLeft" activeCell="E82" sqref="E80:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5190,7 +5190,7 @@
         <v>101</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>17</v>
@@ -5210,7 +5210,7 @@
         <v>101</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>17</v>
@@ -6430,9 +6430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6920,7 +6920,7 @@
         <v>101</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>44</v>
@@ -13948,7 +13948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
     </sheetView>

</xml_diff>

<commit_message>
Update turkey content status
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F474A557-219E-4479-AFF4-A7FD7BB427D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2239B4FF-8841-49D5-9155-72CC5B1396FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2136,7 +2136,58 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
+  <dxfs count="144">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3589,8 +3640,8 @@
   <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4901,7 +4952,7 @@
         <v>156</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>17</v>
@@ -4921,7 +4972,7 @@
         <v>156</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>17</v>
@@ -4941,7 +4992,7 @@
         <v>156</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>17</v>
@@ -6173,83 +6224,83 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E1:E65 E69:E1048576">
-    <cfRule type="containsText" dxfId="137" priority="25" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="E69:E1048576 E1:E65">
+    <cfRule type="containsText" dxfId="143" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="142" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="141" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="140" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="139" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="138" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" dxfId="131" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="137" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="136" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="135" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="134" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="133" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="132" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="containsText" dxfId="125" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="131" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="130" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="129" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="128" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="127" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="126" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="125" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="124" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="123" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="122" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="121" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="120" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6449,22 +6500,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6483,7 +6534,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7354,7 +7405,7 @@
         <v>156</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>25</v>
@@ -7941,144 +7992,164 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B24 B33 B53:B54 B40:B51 B56:B1048576">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="B1:B24 B33 B53:B54 B40:B49 B56:B1048576 B51">
+    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B50)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -10247,22 +10318,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11293,22 +11364,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13744,42 +13815,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13981,22 +14052,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16147,22 +16218,22 @@
   <autoFilter ref="A1:K69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16660,22 +16731,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16772,62 +16843,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C5:C1048576">
-    <cfRule type="containsText" dxfId="71" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="65" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16932,22 +17003,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Yule Cat content status
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2239B4FF-8841-49D5-9155-72CC5B1396FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B48228-84A1-4743-BF60-4FF65BD24784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -2136,7 +2136,58 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
+  <dxfs count="150">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3639,9 +3690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5212,7 +5263,7 @@
         <v>174</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>17</v>
@@ -6224,83 +6275,83 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E69:E1048576 E1:E65">
-    <cfRule type="containsText" dxfId="143" priority="25" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="E1:E65 E69:E1048576">
+    <cfRule type="containsText" dxfId="149" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="148" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="147" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="146" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="145" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="144" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" dxfId="137" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="143" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="142" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="141" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="140" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="139" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="138" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="containsText" dxfId="131" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="137" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="136" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="135" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="134" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="133" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="132" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="containsText" dxfId="125" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="131" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="130" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="129" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="128" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="127" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="126" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6500,22 +6551,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6532,9 +6583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7482,7 +7533,7 @@
         <v>174</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>25</v>
@@ -7992,164 +8043,184 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B24 B33 B53:B54 B40:B49 B56:B1048576 B51">
-    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="B1:B24 B33 B53 B40:B49 B56:B1048576 B51">
+    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B50)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B54)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Complete",B54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -10318,22 +10389,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="125" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="124" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="123" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="122" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="121" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="120" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11364,22 +11435,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="119" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="118" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="117" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="116" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="115" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="114" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13815,42 +13886,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14052,22 +14123,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16218,22 +16289,22 @@
   <autoFilter ref="A1:K69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16731,22 +16802,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16843,62 +16914,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C5:C1048576">
-    <cfRule type="containsText" dxfId="77" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17003,22 +17074,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update A Wicked Brew content status
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B48228-84A1-4743-BF60-4FF65BD24784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8CA34F-81B6-42E3-9F3C-90943725E633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -2136,7 +2136,160 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="150">
+  <dxfs count="168">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6276,82 +6429,82 @@
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E1:E65 E69:E1048576">
-    <cfRule type="containsText" dxfId="149" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="167" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="166" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="165" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="164" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="163" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="162" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" dxfId="143" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="161" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="160" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="159" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="158" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="157" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="156" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="containsText" dxfId="137" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="155" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="154" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="153" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="152" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="151" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="150" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="containsText" dxfId="131" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="149" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="148" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="147" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="146" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="145" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="144" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E68)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6465,9 +6618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6505,7 +6658,7 @@
         <v>181</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -6550,24 +6703,44 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="C1 C3:C1048576">
+    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -6583,9 +6756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7593,7 +7766,7 @@
         <v>181</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>25</v>
@@ -7732,7 +7905,7 @@
         <v>253</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>44</v>
@@ -8043,184 +8216,224 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B24 B33 B53 B40:B49 B56:B1048576 B51">
-    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="B1:B24 B33 B53 B40:B49 B56 B51 B58:B64 B66:B1048576">
+    <cfRule type="containsText" dxfId="71" priority="61" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="62" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="63" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B32">
-    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="55" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="56" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="57" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="58" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="49" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="50" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="51" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="43" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="44" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B39">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="37" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="38" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="31" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="32" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Playtest Ready">
+      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Needs Clean Up">
+      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Needs Review">
+      <formula>NOT(ISERROR(SEARCH("Needs Review",B65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -8316,7 +8529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10389,22 +10602,22 @@
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="125" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="143" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="142" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="141" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="140" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="139" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="138" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11435,22 +11648,22 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="119" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="137" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="136" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="135" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="134" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="133" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="132" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13886,42 +14099,42 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="131" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="130" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="129" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="128" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="127" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="126" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="125" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="124" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="123" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="122" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="121" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="120" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14123,22 +14336,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="101" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16289,22 +16502,22 @@
   <autoFilter ref="A1:K69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="111" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="110" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="109" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="108" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16802,22 +17015,22 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16914,62 +17127,62 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C5:C1048576">
-    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17074,22 +17287,22 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update review status of mishipeshu and water stallion
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46502C1-028E-406A-9C47-D0EB38E01F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FECDEE-DCB2-4005-A76C-559C10E10DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -3843,9 +3843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5276,7 +5276,7 @@
         <v>164</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>17</v>
@@ -5416,7 +5416,7 @@
         <v>174</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>17</v>
@@ -5436,7 +5436,7 @@
         <v>175</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>17</v>
@@ -5456,7 +5456,7 @@
         <v>175</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>17</v>
@@ -5476,7 +5476,7 @@
         <v>175</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>17</v>
@@ -6428,7 +6428,7 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E1:E65 E69:E1048576">
+  <conditionalFormatting sqref="E1:E65 E70:E1048576">
     <cfRule type="containsText" dxfId="167" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
@@ -6488,7 +6488,7 @@
       <formula>NOT(ISERROR(SEARCH("Complete",E67)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+  <conditionalFormatting sqref="E68:E69">
     <cfRule type="containsText" dxfId="149" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E68)))</formula>
     </cfRule>
@@ -6756,9 +6756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B79:B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7669,7 +7669,7 @@
         <v>164</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>44</v>
@@ -7726,7 +7726,7 @@
         <v>175</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>25</v>
@@ -8216,7 +8216,7 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B24 B33 B53 B40:B49 B56 B51 B58:B64 B66:B1048576">
+  <conditionalFormatting sqref="B1:B24 B33 B40:B49 B58:B64 B66:B1048576 B55:B56 B51:B53">
     <cfRule type="containsText" dxfId="65" priority="61" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
@@ -8314,46 +8314,6 @@
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Playtest Ready">
-      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Needs Clean Up">
-      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",B52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B55">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Playtest Ready">
-      <formula>NOT(ISERROR(SEARCH("Playtest Ready",B55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Needs Clean Up">
-      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",B55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">

</xml_diff>

<commit_message>
Release spike fists and update content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090E6438-44B6-45EA-865C-84F061053B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106A6F93-FFF2-4FCB-AE39-031E69D02918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3591" uniqueCount="643">
   <si>
     <t>Name</t>
   </si>
@@ -1998,6 +1998,15 @@
   </si>
   <si>
     <t>Humanoid (ratfolk)</t>
+  </si>
+  <si>
+    <t>Terlen</t>
+  </si>
+  <si>
+    <t>Terlens</t>
+  </si>
+  <si>
+    <t>Spike Fists</t>
   </si>
 </sst>
 </file>
@@ -3784,11 +3793,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D128" sqref="D128"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6405,6 +6414,26 @@
         <v>14</v>
       </c>
       <c r="F128" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B129" s="7">
+        <v>4</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F129" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6593,9 +6622,10 @@
     <hyperlink ref="D126" r:id="rId99" xr:uid="{8FD7497B-7CAD-4106-9444-6EDC680D286F}"/>
     <hyperlink ref="D127" r:id="rId100" xr:uid="{51D6B55B-7477-4DB7-853B-8D3C295F6E7C}"/>
     <hyperlink ref="D128" r:id="rId101" xr:uid="{E0A10021-8039-4BEF-ABE5-1C5A8E55CF77}"/>
+    <hyperlink ref="D129" r:id="rId102" xr:uid="{E138BAFE-12C4-4023-8FD7-504DDB9828F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId102"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId103"/>
 </worksheet>
 </file>
 
@@ -6727,11 +6757,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8251,6 +8281,40 @@
       </c>
       <c r="E86" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -8542,9 +8606,11 @@
     <hyperlink ref="A84" r:id="rId83" xr:uid="{53AB8ED9-F49B-4AF1-A35E-A98942D8268D}"/>
     <hyperlink ref="A85" r:id="rId84" xr:uid="{C35F06FF-3879-43BE-8EC5-313ECD2C9BC7}"/>
     <hyperlink ref="A86" r:id="rId85" xr:uid="{51114850-F39C-40B2-B1B9-8E2950FD4D56}"/>
+    <hyperlink ref="A87" r:id="rId86" xr:uid="{8ACF3EB5-AE7C-4D41-91FC-234B26E1ED03}"/>
+    <hyperlink ref="A88" r:id="rId87" xr:uid="{28048917-5FE2-4CD1-982E-16F7BA9FC041}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId86"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId88"/>
 </worksheet>
 </file>
 
@@ -8552,8 +8618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -14184,7 +14250,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14344,10 +14410,10 @@
         <v>338</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add primeval fish to content sheet
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468C003D-BDEF-4D64-80F4-C16962F9184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE04C5C-D1E2-4804-A75E-DFE61F7C7613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3591" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="646">
   <si>
     <t>Name</t>
   </si>
@@ -2007,6 +2007,15 @@
   </si>
   <si>
     <t>Spike Fists</t>
+  </si>
+  <si>
+    <t>Dunkleosteus</t>
+  </si>
+  <si>
+    <t>Megalodon</t>
+  </si>
+  <si>
+    <t>Primeval Fish</t>
   </si>
 </sst>
 </file>
@@ -3793,11 +3802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6434,6 +6443,46 @@
         <v>14</v>
       </c>
       <c r="F129" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B130" s="7">
+        <v>6</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B131" s="7">
+        <v>10</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6623,9 +6672,11 @@
     <hyperlink ref="D127" r:id="rId100" xr:uid="{51D6B55B-7477-4DB7-853B-8D3C295F6E7C}"/>
     <hyperlink ref="D128" r:id="rId101" xr:uid="{E0A10021-8039-4BEF-ABE5-1C5A8E55CF77}"/>
     <hyperlink ref="D129" r:id="rId102" xr:uid="{E138BAFE-12C4-4023-8FD7-504DDB9828F7}"/>
+    <hyperlink ref="D130" r:id="rId103" xr:uid="{CFFAF4FE-9C8F-42EF-8A76-8C176AB3850D}"/>
+    <hyperlink ref="D131" r:id="rId104" xr:uid="{F678843D-DF87-492B-9A3A-FA0B724BD233}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId103"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId105"/>
 </worksheet>
 </file>
 
@@ -6757,11 +6808,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8315,6 +8366,23 @@
       </c>
       <c r="E88" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8608,9 +8676,10 @@
     <hyperlink ref="A86" r:id="rId85" xr:uid="{51114850-F39C-40B2-B1B9-8E2950FD4D56}"/>
     <hyperlink ref="A87" r:id="rId86" xr:uid="{8ACF3EB5-AE7C-4D41-91FC-234B26E1ED03}"/>
     <hyperlink ref="A88" r:id="rId87" xr:uid="{28048917-5FE2-4CD1-982E-16F7BA9FC041}"/>
+    <hyperlink ref="A89" r:id="rId88" xr:uid="{9BF6D558-ED8C-438D-9E61-2F3083B8D992}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId88"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId89"/>
 </worksheet>
 </file>
 
@@ -8618,7 +8687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>

</xml_diff>

<commit_message>
Add Umibozu to content lists
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67ABF35-86B7-4E60-BBC2-A92A5A832AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD775A-0EE9-4B06-8E57-EBE9F9C04C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4060" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="714">
   <si>
     <t>Name</t>
   </si>
@@ -2214,6 +2214,12 @@
   </si>
   <si>
     <t>Angler Mimic</t>
+  </si>
+  <si>
+    <t>Umibōzu</t>
+  </si>
+  <si>
+    <t>Undead</t>
   </si>
 </sst>
 </file>
@@ -2361,568 +2367,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="162">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="96">
     <dxf>
       <fill>
         <patternFill>
@@ -4015,11 +3460,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F89" sqref="F42:F89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7192,26 +6637,49 @@
         <v>16</v>
       </c>
     </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B136" s="7">
+        <v>15</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D136" s="22" t="s">
+        <v>707</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="161" priority="25" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="25" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="26" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="26" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="27" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="27" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="28" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="28" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="29" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="29" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="30" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="30" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7324,9 +6792,10 @@
     <hyperlink ref="E133" r:id="rId106" xr:uid="{D74B88D5-C25E-46C0-AA60-A9E139A1D406}"/>
     <hyperlink ref="E134" r:id="rId107" xr:uid="{0859541D-9598-49BB-A701-650BBBB662A4}"/>
     <hyperlink ref="E135" r:id="rId108" xr:uid="{2A88B4B0-9CAE-4ADD-ACDC-EF8466C5C57C}"/>
+    <hyperlink ref="E136" r:id="rId109" xr:uid="{79054CA5-E564-4750-ADFC-7A8CD2DE7E00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId109"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId110"/>
 </worksheet>
 </file>
 
@@ -7430,42 +6899,42 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="D1 D4:D1048576">
-    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7480,11 +6949,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9131,46 +8600,63 @@
         <v>1</v>
       </c>
     </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B58:B1048576 B1:B55">
-    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="B1:B55 B58:B1048576">
+    <cfRule type="containsText" dxfId="17" priority="67" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="68" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="68" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="69" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="69" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="70" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="70" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="71" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="71" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="72" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="72" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9287,9 +8773,10 @@
     <hyperlink ref="A91" r:id="rId90" xr:uid="{51175513-C304-43DA-85E8-8CF1FDC59235}"/>
     <hyperlink ref="A92" r:id="rId91" xr:uid="{530F211E-57DA-4A7A-8BB9-D73E949C9080}"/>
     <hyperlink ref="A93" r:id="rId92" xr:uid="{DC430166-709F-4CA8-9813-605C406F2A3E}"/>
+    <hyperlink ref="A94" r:id="rId93" xr:uid="{3E9A8FCA-6B45-4D15-BAF0-FD0AFDB2F4A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId93"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId94"/>
 </worksheet>
 </file>
 
@@ -9385,42 +8872,42 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C5:C1048576">
-    <cfRule type="containsText" dxfId="137" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="85" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="131" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11516,22 +11003,22 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="119" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12562,22 +12049,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="113" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13494,22 +12981,22 @@
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="107" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16078,42 +15565,42 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16345,22 +15832,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18754,22 +18241,22 @@
   <autoFilter ref="A1:L69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18874,22 +18361,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add Mummy Lords to content lists
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD775A-0EE9-4B06-8E57-EBE9F9C04C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C7AFC1-09A0-4FA1-9469-AFB797FB4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4082" uniqueCount="716">
   <si>
     <t>Name</t>
   </si>
@@ -2220,6 +2220,12 @@
   </si>
   <si>
     <t>Undead</t>
+  </si>
+  <si>
+    <t>Mummy Lord</t>
+  </si>
+  <si>
+    <t>Desert, Underdark</t>
   </si>
 </sst>
 </file>
@@ -3460,11 +3466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
+      <selection pane="bottomLeft" activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6657,6 +6663,29 @@
         <v>14</v>
       </c>
       <c r="G136" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="B137" s="7">
+        <v>17</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D137" s="22" t="s">
+        <v>715</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G137" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6793,9 +6822,10 @@
     <hyperlink ref="E134" r:id="rId107" xr:uid="{0859541D-9598-49BB-A701-650BBBB662A4}"/>
     <hyperlink ref="E135" r:id="rId108" xr:uid="{2A88B4B0-9CAE-4ADD-ACDC-EF8466C5C57C}"/>
     <hyperlink ref="E136" r:id="rId109" xr:uid="{79054CA5-E564-4750-ADFC-7A8CD2DE7E00}"/>
+    <hyperlink ref="E137" r:id="rId110" xr:uid="{573A7395-469F-444B-9F53-2E831A08FB93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId110"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId111"/>
 </worksheet>
 </file>
 
@@ -6949,11 +6979,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8614,6 +8644,23 @@
         <v>16</v>
       </c>
       <c r="E94" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8774,9 +8821,10 @@
     <hyperlink ref="A92" r:id="rId91" xr:uid="{530F211E-57DA-4A7A-8BB9-D73E949C9080}"/>
     <hyperlink ref="A93" r:id="rId92" xr:uid="{DC430166-709F-4CA8-9813-605C406F2A3E}"/>
     <hyperlink ref="A94" r:id="rId93" xr:uid="{3E9A8FCA-6B45-4D15-BAF0-FD0AFDB2F4A1}"/>
+    <hyperlink ref="A95" r:id="rId94" xr:uid="{28B85654-8FAF-40B2-B666-6F592C7C587D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId94"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId95"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Remove "Any" as environment type for creatures
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD775A-0EE9-4B06-8E57-EBE9F9C04C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B4F93-43BF-4861-8444-135D3D0B82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="716">
   <si>
     <t>Name</t>
   </si>
@@ -2174,9 +2174,6 @@
     <t>Freshwater, Underwater</t>
   </si>
   <si>
-    <t>Any</t>
-  </si>
-  <si>
     <t>Freshwater, Urban</t>
   </si>
   <si>
@@ -2220,6 +2217,15 @@
   </si>
   <si>
     <t>Undead</t>
+  </si>
+  <si>
+    <t>Arctic, Coastal, Desert, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp, Underdark, Underwater, Urban</t>
+  </si>
+  <si>
+    <t>Arctic, Coastal, Desert, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp, Underdark, Underwater</t>
+  </si>
+  <si>
+    <t>Arctic, Coastal, Desert, Extraplanar, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp, Underdark, Underwater, Urban</t>
   </si>
 </sst>
 </file>
@@ -3463,8 +3469,8 @@
   <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,7 +3700,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B9" s="7">
         <v>3</v>
@@ -3798,7 +3804,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B13" s="7">
         <v>17</v>
@@ -3859,7 +3865,7 @@
         <v>132</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>43</v>
@@ -4564,7 +4570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>130</v>
       </c>
@@ -4575,7 +4581,7 @@
         <v>131</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>112</v>
@@ -4587,7 +4593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>133</v>
       </c>
@@ -4598,7 +4604,7 @@
         <v>131</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>112</v>
@@ -4610,7 +4616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>134</v>
       </c>
@@ -4621,7 +4627,7 @@
         <v>131</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>112</v>
@@ -4633,7 +4639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>135</v>
       </c>
@@ -4644,7 +4650,7 @@
         <v>131</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>112</v>
@@ -4656,7 +4662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>136</v>
       </c>
@@ -4667,7 +4673,7 @@
         <v>131</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>115</v>
@@ -4679,7 +4685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>137</v>
       </c>
@@ -4690,7 +4696,7 @@
         <v>131</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>115</v>
@@ -4702,7 +4708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>138</v>
       </c>
@@ -4713,7 +4719,7 @@
         <v>131</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>118</v>
@@ -4725,7 +4731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>139</v>
       </c>
@@ -4736,7 +4742,7 @@
         <v>131</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>118</v>
@@ -4748,7 +4754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>140</v>
       </c>
@@ -4759,7 +4765,7 @@
         <v>131</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>125</v>
@@ -4771,7 +4777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>141</v>
       </c>
@@ -4782,7 +4788,7 @@
         <v>131</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>125</v>
@@ -4794,7 +4800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>142</v>
       </c>
@@ -4805,7 +4811,7 @@
         <v>131</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>698</v>
+        <v>714</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>121</v>
@@ -4817,7 +4823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>143</v>
       </c>
@@ -4828,7 +4834,7 @@
         <v>131</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>698</v>
+        <v>714</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>121</v>
@@ -4851,7 +4857,7 @@
         <v>94</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>144</v>
@@ -4874,7 +4880,7 @@
         <v>147</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>144</v>
@@ -4943,7 +4949,7 @@
         <v>94</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>144</v>
@@ -4978,7 +4984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>153</v>
       </c>
@@ -4989,7 +4995,7 @@
         <v>96</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>698</v>
+        <v>715</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>151</v>
@@ -5001,7 +5007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
@@ -5012,7 +5018,7 @@
         <v>96</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>698</v>
+        <v>715</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>151</v>
@@ -5081,7 +5087,7 @@
         <v>96</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>155</v>
@@ -5104,7 +5110,7 @@
         <v>96</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>159</v>
@@ -5127,7 +5133,7 @@
         <v>94</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>161</v>
@@ -5150,7 +5156,7 @@
         <v>94</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>161</v>
@@ -5173,7 +5179,7 @@
         <v>147</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>161</v>
@@ -5196,7 +5202,7 @@
         <v>166</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>161</v>
@@ -5219,7 +5225,7 @@
         <v>166</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>161</v>
@@ -5242,7 +5248,7 @@
         <v>166</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>161</v>
@@ -5265,7 +5271,7 @@
         <v>95</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>169</v>
@@ -5403,7 +5409,7 @@
         <v>166</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>161</v>
@@ -5426,7 +5432,7 @@
         <v>166</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>161</v>
@@ -5449,7 +5455,7 @@
         <v>180</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>161</v>
@@ -5472,7 +5478,7 @@
         <v>166</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>161</v>
@@ -5495,7 +5501,7 @@
         <v>94</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>248</v>
@@ -5518,7 +5524,7 @@
         <v>94</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>248</v>
@@ -5541,7 +5547,7 @@
         <v>132</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>248</v>
@@ -5564,7 +5570,7 @@
         <v>94</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>292</v>
@@ -5587,7 +5593,7 @@
         <v>94</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>292</v>
@@ -5610,7 +5616,7 @@
         <v>94</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>292</v>
@@ -5633,7 +5639,7 @@
         <v>147</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>292</v>
@@ -5656,7 +5662,7 @@
         <v>147</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>292</v>
@@ -5679,7 +5685,7 @@
         <v>166</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>292</v>
@@ -5702,7 +5708,7 @@
         <v>166</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>315</v>
@@ -5725,7 +5731,7 @@
         <v>166</v>
       </c>
       <c r="D96" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>315</v>
@@ -5751,7 +5757,7 @@
         <v>166</v>
       </c>
       <c r="D97" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>315</v>
@@ -5774,7 +5780,7 @@
         <v>132</v>
       </c>
       <c r="D98" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>315</v>
@@ -5797,7 +5803,7 @@
         <v>132</v>
       </c>
       <c r="D99" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>315</v>
@@ -5820,7 +5826,7 @@
         <v>166</v>
       </c>
       <c r="D100" s="22" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>315</v>
@@ -6004,7 +6010,7 @@
         <v>636</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>349</v>
@@ -6027,7 +6033,7 @@
         <v>636</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>351</v>
@@ -6211,7 +6217,7 @@
         <v>636</v>
       </c>
       <c r="D117" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>618</v>
@@ -6303,7 +6309,7 @@
         <v>94</v>
       </c>
       <c r="D121" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>631</v>
@@ -6326,7 +6332,7 @@
         <v>94</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>631</v>
@@ -6349,7 +6355,7 @@
         <v>94</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>631</v>
@@ -6464,7 +6470,7 @@
         <v>636</v>
       </c>
       <c r="D128" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>635</v>
@@ -6487,7 +6493,7 @@
         <v>166</v>
       </c>
       <c r="D129" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>638</v>
@@ -6556,7 +6562,7 @@
         <v>636</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>643</v>
@@ -6579,7 +6585,7 @@
         <v>166</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>644</v>
@@ -6593,7 +6599,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B134" s="7">
         <v>13</v>
@@ -6602,10 +6608,10 @@
         <v>636</v>
       </c>
       <c r="D134" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>14</v>
@@ -6616,7 +6622,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B135" s="7">
         <v>12</v>
@@ -6628,7 +6634,7 @@
         <v>694</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>14</v>
@@ -6639,19 +6645,19 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B136" s="7">
         <v>15</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D136" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>14</v>
@@ -8565,7 +8571,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>14</v>
@@ -8585,7 +8591,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>14</v>
@@ -8602,7 +8608,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Add vermin lords to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B4F93-43BF-4861-8444-135D3D0B82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295E2F7D-9313-48A0-B1F8-2F71DE7F80C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4071" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4112" uniqueCount="723">
   <si>
     <t>Name</t>
   </si>
@@ -2226,6 +2226,27 @@
   </si>
   <si>
     <t>Arctic, Coastal, Desert, Extraplanar, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp, Underdark, Underwater, Urban</t>
+  </si>
+  <si>
+    <t>Vermin Lord Corruptor</t>
+  </si>
+  <si>
+    <t>Vermin Lord Deceiver</t>
+  </si>
+  <si>
+    <t>Vermin Lord Warbringer</t>
+  </si>
+  <si>
+    <t>Vermin Lord Warpseer</t>
+  </si>
+  <si>
+    <t>Vermin Lords</t>
+  </si>
+  <si>
+    <t>Mummy Lord</t>
+  </si>
+  <si>
+    <t>Desert, Underdark</t>
   </si>
 </sst>
 </file>
@@ -3466,11 +3487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6663,6 +6684,121 @@
         <v>14</v>
       </c>
       <c r="G136" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B137" s="7">
+        <v>16</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D137" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B138" s="7">
+        <v>18</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D138" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B139" s="7">
+        <v>17</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D139" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B140" s="7">
+        <v>19</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D140" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B141" s="7">
+        <v>17</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D141" s="22" t="s">
+        <v>722</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G141" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6799,9 +6935,14 @@
     <hyperlink ref="E134" r:id="rId107" xr:uid="{0859541D-9598-49BB-A701-650BBBB662A4}"/>
     <hyperlink ref="E135" r:id="rId108" xr:uid="{2A88B4B0-9CAE-4ADD-ACDC-EF8466C5C57C}"/>
     <hyperlink ref="E136" r:id="rId109" xr:uid="{79054CA5-E564-4750-ADFC-7A8CD2DE7E00}"/>
+    <hyperlink ref="E137" r:id="rId110" xr:uid="{0140BEFC-24C1-44CB-B044-14AC8D9D7E83}"/>
+    <hyperlink ref="E138" r:id="rId111" xr:uid="{C91F8F74-635B-4E9C-82EA-357BD873EA0D}"/>
+    <hyperlink ref="E139" r:id="rId112" xr:uid="{37D7D39C-E756-4ABA-ACCE-6D6214469C2A}"/>
+    <hyperlink ref="E140" r:id="rId113" xr:uid="{47254F5C-7CA5-4837-91EB-1B1D0C75B690}"/>
+    <hyperlink ref="E141" r:id="rId114" xr:uid="{4813D3FA-EA0C-4EA9-B7E8-9B19993E3991}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId110"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId115"/>
 </worksheet>
 </file>
 
@@ -6955,11 +7096,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8623,66 +8764,103 @@
         <v>1</v>
       </c>
     </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B55 B58:B1048576">
-    <cfRule type="containsText" dxfId="17" priority="67" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="5" priority="67" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="68" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="4" priority="68" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="69" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="69" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="70" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="2" priority="70" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="71" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="1" priority="71" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="72" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="72" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B56)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8780,9 +8958,11 @@
     <hyperlink ref="A92" r:id="rId91" xr:uid="{530F211E-57DA-4A7A-8BB9-D73E949C9080}"/>
     <hyperlink ref="A93" r:id="rId92" xr:uid="{DC430166-709F-4CA8-9813-605C406F2A3E}"/>
     <hyperlink ref="A94" r:id="rId93" xr:uid="{3E9A8FCA-6B45-4D15-BAF0-FD0AFDB2F4A1}"/>
+    <hyperlink ref="A95" r:id="rId94" xr:uid="{5434F518-6AB1-4B01-A88B-4D039A9C3D88}"/>
+    <hyperlink ref="A96" r:id="rId95" xr:uid="{1EA62A18-6667-4477-AD37-4AB796241C4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId94"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId96"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Public Content Compendiums
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A4FE4-B2B7-4160-B89F-4F5B6431EC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99B3E35-9FC6-4360-8859-FDC054F17547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -3696,8 +3696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
@@ -10168,8 +10168,8 @@
   <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16859,8 +16859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACF069B-924A-40FE-91D9-4FC2DC64FE41}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17095,15 +17095,15 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="New Weapons" xr:uid="{CC9F76B0-4120-40E2-8D59-C8EC3C02CBCB}"/>
-    <hyperlink ref="F3" r:id="rId2" display="New Weapons" xr:uid="{307B2ED2-A702-4596-82DF-3468BA8704FF}"/>
-    <hyperlink ref="F4" r:id="rId3" display="New Weapons" xr:uid="{06D6BE93-4FE2-4532-A6F9-A86FF70D4EB6}"/>
-    <hyperlink ref="F5" r:id="rId4" display="New Weapons" xr:uid="{ED541B3E-5B84-4BEA-910F-E5F6E0C86418}"/>
+    <hyperlink ref="F10" r:id="rId1" display="New Weapons" xr:uid="{3D35BBA4-6255-4979-8AB7-547AFF4B3B41}"/>
+    <hyperlink ref="F9" r:id="rId2" display="New Weapons" xr:uid="{6B15E3E7-F401-426A-A18E-57996A25F79A}"/>
+    <hyperlink ref="F8" r:id="rId3" display="New Weapons" xr:uid="{80EC7E2D-14E4-47D3-BF22-208E0922C7A4}"/>
+    <hyperlink ref="F7" r:id="rId4" display="New Weapons" xr:uid="{87E4731E-CCC3-449A-B3C7-F06415DEC287}"/>
     <hyperlink ref="F6" r:id="rId5" display="New Weapons" xr:uid="{376ECC15-E7A0-4D34-8D39-908D59197911}"/>
-    <hyperlink ref="F7" r:id="rId6" display="New Weapons" xr:uid="{87E4731E-CCC3-449A-B3C7-F06415DEC287}"/>
-    <hyperlink ref="F8" r:id="rId7" display="New Weapons" xr:uid="{80EC7E2D-14E4-47D3-BF22-208E0922C7A4}"/>
-    <hyperlink ref="F9" r:id="rId8" display="New Weapons" xr:uid="{6B15E3E7-F401-426A-A18E-57996A25F79A}"/>
-    <hyperlink ref="F10" r:id="rId9" display="New Weapons" xr:uid="{3D35BBA4-6255-4979-8AB7-547AFF4B3B41}"/>
+    <hyperlink ref="F5" r:id="rId6" display="New Weapons" xr:uid="{ED541B3E-5B84-4BEA-910F-E5F6E0C86418}"/>
+    <hyperlink ref="F4" r:id="rId7" display="New Weapons" xr:uid="{06D6BE93-4FE2-4532-A6F9-A86FF70D4EB6}"/>
+    <hyperlink ref="F3" r:id="rId8" display="New Weapons" xr:uid="{307B2ED2-A702-4596-82DF-3468BA8704FF}"/>
+    <hyperlink ref="F2" r:id="rId9" display="New Weapons" xr:uid="{CC9F76B0-4120-40E2-8D59-C8EC3C02CBCB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17115,7 +17115,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20450,7 +20450,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add wolf, werewolf, and ratfolk content
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99B3E35-9FC6-4360-8859-FDC054F17547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3776655F-4E12-4EF1-90E5-0C650726AB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4639" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4688" uniqueCount="788">
   <si>
     <t>Name</t>
   </si>
@@ -2403,6 +2403,45 @@
   </si>
   <si>
     <t>Ratfolk Volcanic Tailslasher</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Dire Wolf</t>
+  </si>
+  <si>
+    <t>Ascendant Packleader</t>
+  </si>
+  <si>
+    <t>Celestial</t>
+  </si>
+  <si>
+    <t>Arctic, Desert, Forest, Grassland, Hills, Mountain</t>
+  </si>
+  <si>
+    <t>Arctic, Desert, Extraplanar, Forest, Grassland, Hills, Mountain</t>
+  </si>
+  <si>
+    <t>Wolves</t>
+  </si>
+  <si>
+    <t>Werewolf, Lone</t>
+  </si>
+  <si>
+    <t>Werewolf, Pack</t>
+  </si>
+  <si>
+    <t>Werewolf Moon Mystic</t>
+  </si>
+  <si>
+    <t>Werewolf Pack Leader</t>
+  </si>
+  <si>
+    <t>Arctic, Desert, Extraplanar, Forest, Grassland, Hills, Mountain, Urban</t>
+  </si>
+  <si>
+    <t>Werewolves</t>
   </si>
 </sst>
 </file>
@@ -2477,7 +2516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2508,12 +2547,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3694,11 +3727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J156"/>
+  <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F147" sqref="F147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,10 +3740,10 @@
     <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
@@ -3729,7 +3762,7 @@
       <c r="D1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>673</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -3761,7 +3794,7 @@
       <c r="D2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>674</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -3770,7 +3803,7 @@
       <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -3790,7 +3823,7 @@
       <c r="D3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="20" t="s">
         <v>674</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -3799,7 +3832,7 @@
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -3819,7 +3852,7 @@
       <c r="D4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="20" t="s">
         <v>674</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -3828,7 +3861,7 @@
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -3848,7 +3881,7 @@
       <c r="D5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="20" t="s">
         <v>674</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -3857,7 +3890,7 @@
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -3877,7 +3910,7 @@
       <c r="D6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="20" t="s">
         <v>674</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -3886,7 +3919,7 @@
       <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -3906,7 +3939,7 @@
       <c r="D7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="20" t="s">
         <v>674</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -3915,7 +3948,7 @@
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -3935,7 +3968,7 @@
       <c r="D8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>676</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -3944,7 +3977,7 @@
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -3964,7 +3997,7 @@
       <c r="D9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -3973,7 +4006,7 @@
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -3993,7 +4026,7 @@
       <c r="D10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -4002,7 +4035,7 @@
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -4022,7 +4055,7 @@
       <c r="D11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -4031,7 +4064,7 @@
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -4051,7 +4084,7 @@
       <c r="D12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -4060,7 +4093,7 @@
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -4080,7 +4113,7 @@
       <c r="D13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -4089,7 +4122,7 @@
       <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -4109,7 +4142,7 @@
       <c r="D14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -4118,7 +4151,7 @@
       <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -4138,7 +4171,7 @@
       <c r="D15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="20" t="s">
         <v>698</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -4147,7 +4180,7 @@
       <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -4167,7 +4200,7 @@
       <c r="D16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -4176,7 +4209,7 @@
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -4196,7 +4229,7 @@
       <c r="D17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -4205,7 +4238,7 @@
       <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4222,7 +4255,7 @@
       <c r="D18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -4231,7 +4264,7 @@
       <c r="G18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4248,7 +4281,7 @@
       <c r="D19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -4257,7 +4290,7 @@
       <c r="G19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4274,7 +4307,7 @@
       <c r="D20" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -4283,7 +4316,7 @@
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4300,7 +4333,7 @@
       <c r="D21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="20" t="s">
         <v>677</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -4309,7 +4342,7 @@
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4326,7 +4359,7 @@
       <c r="D22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="20" t="s">
         <v>677</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -4335,7 +4368,7 @@
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4352,7 +4385,7 @@
       <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -4361,7 +4394,7 @@
       <c r="G23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4378,7 +4411,7 @@
       <c r="D24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -4387,7 +4420,7 @@
       <c r="G24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4404,7 +4437,7 @@
       <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -4413,7 +4446,7 @@
       <c r="G25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4430,7 +4463,7 @@
       <c r="D26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -4439,7 +4472,7 @@
       <c r="G26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4456,7 +4489,7 @@
       <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="20" t="s">
         <v>679</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -4465,7 +4498,7 @@
       <c r="G27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4482,7 +4515,7 @@
       <c r="D28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -4491,7 +4524,7 @@
       <c r="G28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4508,7 +4541,7 @@
       <c r="D29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -4517,7 +4550,7 @@
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4534,7 +4567,7 @@
       <c r="D30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -4543,7 +4576,7 @@
       <c r="G30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4560,7 +4593,7 @@
       <c r="D31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -4569,7 +4602,7 @@
       <c r="G31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4586,7 +4619,7 @@
       <c r="D32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -4595,7 +4628,7 @@
       <c r="G32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4612,7 +4645,7 @@
       <c r="D33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -4621,7 +4654,7 @@
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4638,7 +4671,7 @@
       <c r="D34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -4647,7 +4680,7 @@
       <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4664,7 +4697,7 @@
       <c r="D35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -4673,7 +4706,7 @@
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4690,7 +4723,7 @@
       <c r="D36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -4699,7 +4732,7 @@
       <c r="G36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4716,7 +4749,7 @@
       <c r="D37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -4725,7 +4758,7 @@
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4742,7 +4775,7 @@
       <c r="D38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="E38" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -4751,7 +4784,7 @@
       <c r="G38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4768,7 +4801,7 @@
       <c r="D39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="20" t="s">
         <v>680</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -4777,7 +4810,7 @@
       <c r="G39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4794,7 +4827,7 @@
       <c r="D40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="20" t="s">
         <v>681</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -4803,7 +4836,7 @@
       <c r="G40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4820,7 +4853,7 @@
       <c r="D41" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="20" t="s">
         <v>692</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -4829,7 +4862,7 @@
       <c r="G41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4846,7 +4879,7 @@
       <c r="D42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F42" s="3" t="s">
@@ -4855,7 +4888,7 @@
       <c r="G42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4872,7 +4905,7 @@
       <c r="D43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -4881,7 +4914,7 @@
       <c r="G43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4898,7 +4931,7 @@
       <c r="D44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E44" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -4907,7 +4940,7 @@
       <c r="G44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4924,7 +4957,7 @@
       <c r="D45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="20" t="s">
         <v>693</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -4933,7 +4966,7 @@
       <c r="G45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4950,7 +4983,7 @@
       <c r="D46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E46" s="22" t="s">
+      <c r="E46" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -4959,7 +4992,7 @@
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4976,7 +5009,7 @@
       <c r="D47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E47" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -4985,7 +5018,7 @@
       <c r="G47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5002,7 +5035,7 @@
       <c r="D48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -5011,7 +5044,7 @@
       <c r="G48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5028,7 +5061,7 @@
       <c r="D49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="E49" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -5037,7 +5070,7 @@
       <c r="G49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5054,7 +5087,7 @@
       <c r="D50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E50" s="22" t="s">
+      <c r="E50" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -5063,7 +5096,7 @@
       <c r="G50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5080,7 +5113,7 @@
       <c r="D51" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="22" t="s">
+      <c r="E51" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -5089,7 +5122,7 @@
       <c r="G51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5106,7 +5139,7 @@
       <c r="D52" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E52" s="22" t="s">
+      <c r="E52" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F52" s="3" t="s">
@@ -5115,7 +5148,7 @@
       <c r="G52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5132,7 +5165,7 @@
       <c r="D53" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E53" s="22" t="s">
+      <c r="E53" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F53" s="3" t="s">
@@ -5141,7 +5174,7 @@
       <c r="G53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5158,7 +5191,7 @@
       <c r="D54" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E54" s="22" t="s">
+      <c r="E54" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -5167,7 +5200,7 @@
       <c r="G54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H54" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5184,7 +5217,7 @@
       <c r="D55" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="E55" s="20" t="s">
         <v>709</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -5193,7 +5226,7 @@
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5210,7 +5243,7 @@
       <c r="D56" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="E56" s="20" t="s">
         <v>710</v>
       </c>
       <c r="F56" s="3" t="s">
@@ -5219,7 +5252,7 @@
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5236,7 +5269,7 @@
       <c r="D57" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="E57" s="20" t="s">
         <v>710</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -5245,7 +5278,7 @@
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5262,7 +5295,7 @@
       <c r="D58" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E58" s="22" t="s">
+      <c r="E58" s="20" t="s">
         <v>694</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -5271,7 +5304,7 @@
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5288,7 +5321,7 @@
       <c r="D59" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E59" s="22" t="s">
+      <c r="E59" s="20" t="s">
         <v>694</v>
       </c>
       <c r="F59" s="3" t="s">
@@ -5297,7 +5330,7 @@
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5314,7 +5347,7 @@
       <c r="D60" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="22" t="s">
+      <c r="E60" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F60" s="3" t="s">
@@ -5323,7 +5356,7 @@
       <c r="G60" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5340,7 +5373,7 @@
       <c r="D61" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="22" t="s">
+      <c r="E61" s="20" t="s">
         <v>692</v>
       </c>
       <c r="F61" s="3" t="s">
@@ -5349,7 +5382,7 @@
       <c r="G61" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="H61" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5366,7 +5399,7 @@
       <c r="D62" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E62" s="22" t="s">
+      <c r="E62" s="20" t="s">
         <v>694</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -5375,7 +5408,7 @@
       <c r="G62" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5392,7 +5425,7 @@
       <c r="D63" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E63" s="22" t="s">
+      <c r="E63" s="20" t="s">
         <v>676</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -5401,7 +5434,7 @@
       <c r="G63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H63" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5418,7 +5451,7 @@
       <c r="D64" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E64" s="22" t="s">
+      <c r="E64" s="20" t="s">
         <v>711</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -5427,7 +5460,7 @@
       <c r="G64" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H64" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5444,7 +5477,7 @@
       <c r="D65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="22" t="s">
+      <c r="E65" s="20" t="s">
         <v>711</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -5453,7 +5486,7 @@
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5470,7 +5503,7 @@
       <c r="D66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E66" s="22" t="s">
+      <c r="E66" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F66" s="3" t="s">
@@ -5479,7 +5512,7 @@
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5496,7 +5529,7 @@
       <c r="D67" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E67" s="22" t="s">
+      <c r="E67" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -5505,7 +5538,7 @@
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="H67" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5522,7 +5555,7 @@
       <c r="D68" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E68" s="22" t="s">
+      <c r="E68" s="20" t="s">
         <v>694</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -5531,7 +5564,7 @@
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="H68" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5548,7 +5581,7 @@
       <c r="D69" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E69" s="22" t="s">
+      <c r="E69" s="20" t="s">
         <v>694</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -5557,7 +5590,7 @@
       <c r="G69" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="H69" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5574,7 +5607,7 @@
       <c r="D70" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="E70" s="20" t="s">
         <v>695</v>
       </c>
       <c r="F70" s="3" t="s">
@@ -5583,7 +5616,7 @@
       <c r="G70" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5600,7 +5633,7 @@
       <c r="D71" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E71" s="20" t="s">
         <v>695</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -5609,7 +5642,7 @@
       <c r="G71" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="H71" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5626,7 +5659,7 @@
       <c r="D72" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E72" s="20" t="s">
         <v>695</v>
       </c>
       <c r="F72" s="3" t="s">
@@ -5635,7 +5668,7 @@
       <c r="G72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="H72" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5652,7 +5685,7 @@
       <c r="D73" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E73" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -5661,7 +5694,7 @@
       <c r="G73" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="H73" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5678,7 +5711,7 @@
       <c r="D74" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E74" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F74" s="3" t="s">
@@ -5687,7 +5720,7 @@
       <c r="G74" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5704,7 +5737,7 @@
       <c r="D75" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E75" s="22" t="s">
+      <c r="E75" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F75" s="3" t="s">
@@ -5713,7 +5746,7 @@
       <c r="G75" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5730,7 +5763,7 @@
       <c r="D76" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="22" t="s">
+      <c r="E76" s="20" t="s">
         <v>697</v>
       </c>
       <c r="F76" s="3" t="s">
@@ -5739,7 +5772,7 @@
       <c r="G76" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H76" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5756,7 +5789,7 @@
       <c r="D77" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E77" s="22" t="s">
+      <c r="E77" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F77" s="3" t="s">
@@ -5765,7 +5798,7 @@
       <c r="G77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H77" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5782,7 +5815,7 @@
       <c r="D78" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E78" s="22" t="s">
+      <c r="E78" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -5791,7 +5824,7 @@
       <c r="G78" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5808,7 +5841,7 @@
       <c r="D79" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E79" s="22" t="s">
+      <c r="E79" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F79" s="3" t="s">
@@ -5817,7 +5850,7 @@
       <c r="G79" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H79" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5834,7 +5867,7 @@
       <c r="D80" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E80" s="22" t="s">
+      <c r="E80" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F80" s="3" t="s">
@@ -5843,7 +5876,7 @@
       <c r="G80" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H80" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5860,7 +5893,7 @@
       <c r="D81" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E81" s="22" t="s">
+      <c r="E81" s="20" t="s">
         <v>678</v>
       </c>
       <c r="F81" s="3" t="s">
@@ -5869,7 +5902,7 @@
       <c r="G81" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5886,7 +5919,7 @@
       <c r="D82" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E82" s="22" t="s">
+      <c r="E82" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F82" s="3" t="s">
@@ -5895,7 +5928,7 @@
       <c r="G82" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H82" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5912,7 +5945,7 @@
       <c r="D83" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E83" s="22" t="s">
+      <c r="E83" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F83" s="3" t="s">
@@ -5921,7 +5954,7 @@
       <c r="G83" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H83" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5938,7 +5971,7 @@
       <c r="D84" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E84" s="22" t="s">
+      <c r="E84" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F84" s="3" t="s">
@@ -5947,7 +5980,7 @@
       <c r="G84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H84" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5964,7 +5997,7 @@
       <c r="D85" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E85" s="22" t="s">
+      <c r="E85" s="20" t="s">
         <v>696</v>
       </c>
       <c r="F85" s="3" t="s">
@@ -5973,7 +6006,7 @@
       <c r="G85" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="H85" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5990,7 +6023,7 @@
       <c r="D86" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E86" s="22" t="s">
+      <c r="E86" s="20" t="s">
         <v>699</v>
       </c>
       <c r="F86" s="3" t="s">
@@ -5999,7 +6032,7 @@
       <c r="G86" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H86" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6016,7 +6049,7 @@
       <c r="D87" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E87" s="22" t="s">
+      <c r="E87" s="20" t="s">
         <v>699</v>
       </c>
       <c r="F87" s="3" t="s">
@@ -6025,7 +6058,7 @@
       <c r="G87" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H87" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6042,7 +6075,7 @@
       <c r="D88" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E88" s="22" t="s">
+      <c r="E88" s="20" t="s">
         <v>699</v>
       </c>
       <c r="F88" s="3" t="s">
@@ -6051,7 +6084,7 @@
       <c r="G88" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H88" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6068,7 +6101,7 @@
       <c r="D89" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E89" s="22" t="s">
+      <c r="E89" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F89" s="3" t="s">
@@ -6077,7 +6110,7 @@
       <c r="G89" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H89" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6094,7 +6127,7 @@
       <c r="D90" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E90" s="22" t="s">
+      <c r="E90" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F90" s="3" t="s">
@@ -6103,7 +6136,7 @@
       <c r="G90" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="H90" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6120,7 +6153,7 @@
       <c r="D91" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E91" s="22" t="s">
+      <c r="E91" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F91" s="3" t="s">
@@ -6129,7 +6162,7 @@
       <c r="G91" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="H91" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6146,7 +6179,7 @@
       <c r="D92" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E92" s="22" t="s">
+      <c r="E92" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F92" s="3" t="s">
@@ -6155,7 +6188,7 @@
       <c r="G92" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="H92" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6172,7 +6205,7 @@
       <c r="D93" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E93" s="22" t="s">
+      <c r="E93" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F93" s="3" t="s">
@@ -6181,7 +6214,7 @@
       <c r="G93" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="H93" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6198,7 +6231,7 @@
       <c r="D94" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E94" s="22" t="s">
+      <c r="E94" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F94" s="3" t="s">
@@ -6207,7 +6240,7 @@
       <c r="G94" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H94" s="2" t="s">
+      <c r="H94" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6224,7 +6257,7 @@
       <c r="D95" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E95" s="22" t="s">
+      <c r="E95" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F95" s="3" t="s">
@@ -6233,7 +6266,7 @@
       <c r="G95" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="H95" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6250,7 +6283,7 @@
       <c r="D96" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E96" s="22" t="s">
+      <c r="E96" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F96" s="3" t="s">
@@ -6259,7 +6292,7 @@
       <c r="G96" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="H96" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I96" s="1" t="s">
@@ -6279,7 +6312,7 @@
       <c r="D97" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E97" s="22" t="s">
+      <c r="E97" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F97" s="3" t="s">
@@ -6288,7 +6321,7 @@
       <c r="G97" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="H97" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6305,7 +6338,7 @@
       <c r="D98" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E98" s="22" t="s">
+      <c r="E98" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F98" s="3" t="s">
@@ -6314,7 +6347,7 @@
       <c r="G98" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="H98" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6331,7 +6364,7 @@
       <c r="D99" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E99" s="22" t="s">
+      <c r="E99" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -6340,7 +6373,7 @@
       <c r="G99" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="H99" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6357,7 +6390,7 @@
       <c r="D100" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E100" s="22" t="s">
+      <c r="E100" s="20" t="s">
         <v>701</v>
       </c>
       <c r="F100" s="3" t="s">
@@ -6366,7 +6399,7 @@
       <c r="G100" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="H100" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6383,7 +6416,7 @@
       <c r="D101" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E101" s="22" t="s">
+      <c r="E101" s="20" t="s">
         <v>693</v>
       </c>
       <c r="F101" s="3" t="s">
@@ -6392,7 +6425,7 @@
       <c r="G101" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H101" s="2" t="s">
+      <c r="H101" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6409,7 +6442,7 @@
       <c r="D102" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E102" s="22" t="s">
+      <c r="E102" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F102" s="3" t="s">
@@ -6418,7 +6451,7 @@
       <c r="G102" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="H102" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6435,7 +6468,7 @@
       <c r="D103" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E103" s="22" t="s">
+      <c r="E103" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F103" s="3" t="s">
@@ -6444,7 +6477,7 @@
       <c r="G103" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="H103" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6461,7 +6494,7 @@
       <c r="D104" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E104" s="22" t="s">
+      <c r="E104" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F104" s="3" t="s">
@@ -6470,7 +6503,7 @@
       <c r="G104" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="H104" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6487,7 +6520,7 @@
       <c r="D105" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E105" s="22" t="s">
+      <c r="E105" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F105" s="3" t="s">
@@ -6496,7 +6529,7 @@
       <c r="G105" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="H105" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6513,7 +6546,7 @@
       <c r="D106" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E106" s="22" t="s">
+      <c r="E106" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F106" s="3" t="s">
@@ -6522,7 +6555,7 @@
       <c r="G106" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="H106" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6539,7 +6572,7 @@
       <c r="D107" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E107" s="22" t="s">
+      <c r="E107" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F107" s="3" t="s">
@@ -6548,7 +6581,7 @@
       <c r="G107" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H107" s="2" t="s">
+      <c r="H107" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6565,7 +6598,7 @@
       <c r="D108" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E108" s="22" t="s">
+      <c r="E108" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F108" s="3" t="s">
@@ -6574,7 +6607,7 @@
       <c r="G108" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="H108" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6591,7 +6624,7 @@
       <c r="D109" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E109" s="22" t="s">
+      <c r="E109" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F109" s="3" t="s">
@@ -6600,7 +6633,7 @@
       <c r="G109" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H109" s="2" t="s">
+      <c r="H109" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6617,7 +6650,7 @@
       <c r="D110" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E110" s="22" t="s">
+      <c r="E110" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F110" s="3" t="s">
@@ -6626,7 +6659,7 @@
       <c r="G110" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H110" s="2" t="s">
+      <c r="H110" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6643,7 +6676,7 @@
       <c r="D111" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E111" s="22" t="s">
+      <c r="E111" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F111" s="3" t="s">
@@ -6652,7 +6685,7 @@
       <c r="G111" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H111" s="2" t="s">
+      <c r="H111" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6669,7 +6702,7 @@
       <c r="D112" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E112" s="22" t="s">
+      <c r="E112" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F112" s="3" t="s">
@@ -6678,7 +6711,7 @@
       <c r="G112" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="H112" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6695,7 +6728,7 @@
       <c r="D113" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E113" s="22" t="s">
+      <c r="E113" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F113" s="3" t="s">
@@ -6704,7 +6737,7 @@
       <c r="G113" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H113" s="2" t="s">
+      <c r="H113" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6721,7 +6754,7 @@
       <c r="D114" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E114" s="22" t="s">
+      <c r="E114" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F114" s="3" t="s">
@@ -6730,7 +6763,7 @@
       <c r="G114" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="H114" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6747,7 +6780,7 @@
       <c r="D115" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E115" s="22" t="s">
+      <c r="E115" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F115" s="3" t="s">
@@ -6756,7 +6789,7 @@
       <c r="G115" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="2" t="s">
+      <c r="H115" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6773,7 +6806,7 @@
       <c r="D116" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E116" s="22" t="s">
+      <c r="E116" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F116" s="3" t="s">
@@ -6782,7 +6815,7 @@
       <c r="G116" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="H116" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6799,17 +6832,17 @@
       <c r="D117" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E117" s="22" t="s">
+      <c r="E117" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F117" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -6825,7 +6858,7 @@
       <c r="D118" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E118" s="22" t="s">
+      <c r="E118" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F118" s="3" t="s">
@@ -6834,7 +6867,7 @@
       <c r="G118" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="H118" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6851,7 +6884,7 @@
       <c r="D119" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E119" s="22" t="s">
+      <c r="E119" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F119" s="3" t="s">
@@ -6860,7 +6893,7 @@
       <c r="G119" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="H119" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6877,7 +6910,7 @@
       <c r="D120" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E120" s="22" t="s">
+      <c r="E120" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F120" s="3" t="s">
@@ -6886,7 +6919,7 @@
       <c r="G120" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="H120" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6903,7 +6936,7 @@
       <c r="D121" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E121" s="22" t="s">
+      <c r="E121" s="20" t="s">
         <v>702</v>
       </c>
       <c r="F121" s="3" t="s">
@@ -6912,7 +6945,7 @@
       <c r="G121" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H121" s="2" t="s">
+      <c r="H121" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6929,7 +6962,7 @@
       <c r="D122" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E122" s="22" t="s">
+      <c r="E122" s="20" t="s">
         <v>702</v>
       </c>
       <c r="F122" s="3" t="s">
@@ -6938,7 +6971,7 @@
       <c r="G122" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H122" s="2" t="s">
+      <c r="H122" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6955,7 +6988,7 @@
       <c r="D123" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E123" s="22" t="s">
+      <c r="E123" s="20" t="s">
         <v>702</v>
       </c>
       <c r="F123" s="3" t="s">
@@ -6964,7 +6997,7 @@
       <c r="G123" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="H123" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6981,7 +7014,7 @@
       <c r="D124" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E124" s="22" t="s">
+      <c r="E124" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F124" s="3" t="s">
@@ -6990,7 +7023,7 @@
       <c r="G124" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="H124" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7007,7 +7040,7 @@
       <c r="D125" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E125" s="22" t="s">
+      <c r="E125" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F125" s="3" t="s">
@@ -7016,7 +7049,7 @@
       <c r="G125" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="H125" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7033,7 +7066,7 @@
       <c r="D126" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E126" s="22" t="s">
+      <c r="E126" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F126" s="3" t="s">
@@ -7042,7 +7075,7 @@
       <c r="G126" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="H126" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7059,7 +7092,7 @@
       <c r="D127" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E127" s="22" t="s">
+      <c r="E127" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F127" s="3" t="s">
@@ -7068,7 +7101,7 @@
       <c r="G127" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="H127" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7085,17 +7118,17 @@
       <c r="D128" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E128" s="22" t="s">
+      <c r="E128" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -7111,7 +7144,7 @@
       <c r="D129" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E129" s="22" t="s">
+      <c r="E129" s="20" t="s">
         <v>702</v>
       </c>
       <c r="F129" s="3" t="s">
@@ -7120,7 +7153,7 @@
       <c r="G129" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="H129" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7137,7 +7170,7 @@
       <c r="D130" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E130" s="22" t="s">
+      <c r="E130" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F130" s="3" t="s">
@@ -7146,7 +7179,7 @@
       <c r="G130" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H130" s="2" t="s">
+      <c r="H130" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7163,7 +7196,7 @@
       <c r="D131" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E131" s="22" t="s">
+      <c r="E131" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F131" s="3" t="s">
@@ -7172,7 +7205,7 @@
       <c r="G131" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H131" s="2" t="s">
+      <c r="H131" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7189,17 +7222,17 @@
       <c r="D132" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E132" s="22" t="s">
+      <c r="E132" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H132" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -7215,7 +7248,7 @@
       <c r="D133" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E133" s="22" t="s">
+      <c r="E133" s="20" t="s">
         <v>702</v>
       </c>
       <c r="F133" s="3" t="s">
@@ -7224,7 +7257,7 @@
       <c r="G133" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H133" s="2" t="s">
+      <c r="H133" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7241,7 +7274,7 @@
       <c r="D134" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E134" s="22" t="s">
+      <c r="E134" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F134" s="3" t="s">
@@ -7250,7 +7283,7 @@
       <c r="G134" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H134" s="2" t="s">
+      <c r="H134" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7267,7 +7300,7 @@
       <c r="D135" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E135" s="22" t="s">
+      <c r="E135" s="20" t="s">
         <v>690</v>
       </c>
       <c r="F135" s="3" t="s">
@@ -7276,7 +7309,7 @@
       <c r="G135" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H135" s="2" t="s">
+      <c r="H135" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7293,7 +7326,7 @@
       <c r="D136" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="E136" s="22" t="s">
+      <c r="E136" s="20" t="s">
         <v>702</v>
       </c>
       <c r="F136" s="3" t="s">
@@ -7302,7 +7335,7 @@
       <c r="G136" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H136" s="2" t="s">
+      <c r="H136" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7319,7 +7352,7 @@
       <c r="D137" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E137" s="22" t="s">
+      <c r="E137" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F137" s="3" t="s">
@@ -7328,7 +7361,7 @@
       <c r="G137" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H137" s="2" t="s">
+      <c r="H137" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7345,7 +7378,7 @@
       <c r="D138" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E138" s="22" t="s">
+      <c r="E138" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F138" s="3" t="s">
@@ -7354,7 +7387,7 @@
       <c r="G138" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H138" s="2" t="s">
+      <c r="H138" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7371,7 +7404,7 @@
       <c r="D139" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E139" s="22" t="s">
+      <c r="E139" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F139" s="3" t="s">
@@ -7380,7 +7413,7 @@
       <c r="G139" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H139" s="2" t="s">
+      <c r="H139" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7397,7 +7430,7 @@
       <c r="D140" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E140" s="22" t="s">
+      <c r="E140" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F140" s="3" t="s">
@@ -7406,7 +7439,7 @@
       <c r="G140" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H140" s="2" t="s">
+      <c r="H140" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7423,7 +7456,7 @@
       <c r="D141" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="E141" s="22" t="s">
+      <c r="E141" s="20" t="s">
         <v>718</v>
       </c>
       <c r="F141" s="3" t="s">
@@ -7432,7 +7465,7 @@
       <c r="G141" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H141" s="2" t="s">
+      <c r="H141" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7449,7 +7482,7 @@
       <c r="D142" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E142" s="22" t="s">
+      <c r="E142" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F142" s="3" t="s">
@@ -7458,7 +7491,7 @@
       <c r="G142" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H142" s="2" t="s">
+      <c r="H142" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7475,7 +7508,7 @@
       <c r="D143" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E143" s="22" t="s">
+      <c r="E143" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F143" s="3" t="s">
@@ -7484,7 +7517,7 @@
       <c r="G143" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H143" s="2" t="s">
+      <c r="H143" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7501,7 +7534,7 @@
       <c r="D144" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E144" s="22" t="s">
+      <c r="E144" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F144" s="3" t="s">
@@ -7510,7 +7543,7 @@
       <c r="G144" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H144" s="2" t="s">
+      <c r="H144" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7527,7 +7560,7 @@
       <c r="D145" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E145" s="22" t="s">
+      <c r="E145" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F145" s="3" t="s">
@@ -7536,7 +7569,7 @@
       <c r="G145" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H145" s="2" t="s">
+      <c r="H145" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7553,7 +7586,7 @@
       <c r="D146" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E146" s="22" t="s">
+      <c r="E146" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F146" s="3" t="s">
@@ -7562,7 +7595,7 @@
       <c r="G146" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H146" s="2" t="s">
+      <c r="H146" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7579,7 +7612,7 @@
       <c r="D147" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E147" s="22" t="s">
+      <c r="E147" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F147" s="3" t="s">
@@ -7588,7 +7621,7 @@
       <c r="G147" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H147" s="2" t="s">
+      <c r="H147" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7605,7 +7638,7 @@
       <c r="D148" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E148" s="22" t="s">
+      <c r="E148" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F148" s="3" t="s">
@@ -7614,7 +7647,7 @@
       <c r="G148" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H148" s="2" t="s">
+      <c r="H148" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7631,7 +7664,7 @@
       <c r="D149" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E149" s="22" t="s">
+      <c r="E149" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F149" s="3" t="s">
@@ -7640,7 +7673,7 @@
       <c r="G149" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H149" s="2" t="s">
+      <c r="H149" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7657,17 +7690,17 @@
       <c r="D150" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E150" s="22" t="s">
+      <c r="E150" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F150" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -7683,17 +7716,17 @@
       <c r="D151" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E151" s="22" t="s">
+      <c r="E151" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H151" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -7709,7 +7742,7 @@
       <c r="D152" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E152" s="22" t="s">
+      <c r="E152" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F152" s="3" t="s">
@@ -7718,7 +7751,7 @@
       <c r="G152" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H152" s="2" t="s">
+      <c r="H152" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7735,7 +7768,7 @@
       <c r="D153" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E153" s="22" t="s">
+      <c r="E153" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F153" s="3" t="s">
@@ -7744,7 +7777,7 @@
       <c r="G153" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H153" s="2" t="s">
+      <c r="H153" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7761,7 +7794,7 @@
       <c r="D154" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E154" s="22" t="s">
+      <c r="E154" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F154" s="3" t="s">
@@ -7770,7 +7803,7 @@
       <c r="G154" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H154" s="2" t="s">
+      <c r="H154" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7787,7 +7820,7 @@
       <c r="D155" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E155" s="22" t="s">
+      <c r="E155" s="20" t="s">
         <v>700</v>
       </c>
       <c r="F155" s="3" t="s">
@@ -7796,7 +7829,7 @@
       <c r="G155" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H155" s="2" t="s">
+      <c r="H155" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7813,17 +7846,199 @@
       <c r="D156" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E156" s="22" t="s">
+      <c r="E156" s="20" t="s">
         <v>754</v>
       </c>
       <c r="F156" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H156" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C157" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E157" s="20" t="s">
+        <v>779</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C158" s="7">
+        <v>1</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E158" s="20" t="s">
+        <v>779</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C159" s="7">
+        <v>5</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E159" s="20" t="s">
+        <v>780</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C160" s="7">
+        <v>3</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E160" s="20" t="s">
+        <v>786</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C161" s="7">
+        <v>3</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E161" s="20" t="s">
+        <v>786</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C162" s="7">
+        <v>5</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E162" s="20" t="s">
+        <v>786</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C163" s="7">
+        <v>6</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E163" s="20" t="s">
+        <v>786</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -7833,7 +8048,7 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="G1:G141 G157:G1048576">
+  <conditionalFormatting sqref="G164:G1048576 G1:G141">
     <cfRule type="containsText" dxfId="101" priority="31" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",G1)))</formula>
     </cfRule>
@@ -7853,7 +8068,7 @@
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G142:G156">
+  <conditionalFormatting sqref="G142:G163">
     <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",G142)))</formula>
     </cfRule>
@@ -7997,9 +8212,13 @@
     <hyperlink ref="F151" r:id="rId121" xr:uid="{1C2C13A7-C726-45D0-AAEC-97846CB404CC}"/>
     <hyperlink ref="F153" r:id="rId122" xr:uid="{CFB2A4C0-08D7-4D71-8881-54532EA85CD5}"/>
     <hyperlink ref="F156" r:id="rId123" xr:uid="{DCDDD880-FBDF-40EE-B263-A9B9E27DD194}"/>
+    <hyperlink ref="F157" r:id="rId124" xr:uid="{9A24658D-7A80-492A-9C8C-9947E3042B4F}"/>
+    <hyperlink ref="F158:F159" r:id="rId125" display="Wolves" xr:uid="{2C50CB26-3E8A-4828-A1B0-D4F70F9F7990}"/>
+    <hyperlink ref="F160" r:id="rId126" xr:uid="{B906B306-9128-44E1-8E69-FC114E9C35E6}"/>
+    <hyperlink ref="F161:F163" r:id="rId127" display="Werewolves" xr:uid="{8E85D40E-7B6E-4110-B17F-5A5F4B5A94F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId124"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId128"/>
 </worksheet>
 </file>
 
@@ -8015,7 +8234,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="17" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" style="1" bestFit="1" customWidth="1"/>
@@ -8027,7 +8246,7 @@
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>653</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -8047,7 +8266,7 @@
       <c r="A2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>654</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -8067,7 +8286,7 @@
       <c r="A3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>655</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -8156,7 +8375,7 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
@@ -10039,7 +10258,7 @@
     <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -10054,7 +10273,7 @@
       <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="9" t="s">
@@ -14276,7 +14495,7 @@
   <cols>
     <col min="1" max="1" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -14289,8 +14508,8 @@
     <col min="13" max="13" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="15" customWidth="1"/>
-    <col min="17" max="17" width="8" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="8" style="14" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -14299,10 +14518,10 @@
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>185</v>
       </c>
       <c r="D1" s="10" t="s">
@@ -14338,16 +14557,16 @@
       <c r="N1" s="9" t="s">
         <v>642</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="15" t="s">
         <v>521</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="15" t="s">
         <v>522</v>
       </c>
     </row>
@@ -14358,7 +14577,7 @@
       <c r="B2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -14397,7 +14616,7 @@
       <c r="O2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14408,7 +14627,7 @@
       <c r="B3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="14">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -14447,7 +14666,7 @@
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14458,7 +14677,7 @@
       <c r="B4" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -14497,7 +14716,7 @@
       <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -14508,7 +14727,7 @@
       <c r="B5" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -14547,7 +14766,7 @@
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="P5" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -14558,7 +14777,7 @@
       <c r="B6" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="14">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -14597,7 +14816,7 @@
       <c r="O6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -14608,7 +14827,7 @@
       <c r="B7" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="14">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -14647,7 +14866,7 @@
       <c r="O7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14658,7 +14877,7 @@
       <c r="B8" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -14697,7 +14916,7 @@
       <c r="O8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14708,7 +14927,7 @@
       <c r="B9" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -14747,7 +14966,7 @@
       <c r="O9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="P9" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14758,7 +14977,7 @@
       <c r="B10" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="14">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -14797,7 +15016,7 @@
       <c r="O10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14808,7 +15027,7 @@
       <c r="B11" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -14847,7 +15066,7 @@
       <c r="O11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14858,7 +15077,7 @@
       <c r="B12" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -14897,7 +15116,7 @@
       <c r="O12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="P12" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14908,7 +15127,7 @@
       <c r="B13" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -14947,7 +15166,7 @@
       <c r="O13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="P13" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -14958,7 +15177,7 @@
       <c r="B14" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -14997,7 +15216,7 @@
       <c r="O14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15008,7 +15227,7 @@
       <c r="B15" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="14">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -15047,7 +15266,7 @@
       <c r="O15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="15" t="s">
+      <c r="P15" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15058,7 +15277,7 @@
       <c r="B16" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="14">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -15097,7 +15316,7 @@
       <c r="O16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="P16" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15108,7 +15327,7 @@
       <c r="B17" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="14">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -15147,7 +15366,7 @@
       <c r="O17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P17" s="15" t="s">
+      <c r="P17" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15158,7 +15377,7 @@
       <c r="B18" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="14">
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -15197,7 +15416,7 @@
       <c r="O18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15208,7 +15427,7 @@
       <c r="B19" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="14">
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -15247,7 +15466,7 @@
       <c r="O19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P19" s="15" t="s">
+      <c r="P19" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15258,7 +15477,7 @@
       <c r="B20" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="14">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -15297,7 +15516,7 @@
       <c r="O20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P20" s="15" t="s">
+      <c r="P20" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15308,7 +15527,7 @@
       <c r="B21" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="14">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -15347,7 +15566,7 @@
       <c r="O21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P21" s="15" t="s">
+      <c r="P21" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15358,7 +15577,7 @@
       <c r="B22" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="14">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -15397,7 +15616,7 @@
       <c r="O22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P22" s="15" t="s">
+      <c r="P22" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -15408,7 +15627,7 @@
       <c r="B23" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="14">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -15447,7 +15666,7 @@
       <c r="O23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P23" s="15" t="s">
+      <c r="P23" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -15458,7 +15677,7 @@
       <c r="B24" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="14">
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -15497,7 +15716,7 @@
       <c r="O24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P24" s="15" t="s">
+      <c r="P24" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -15508,7 +15727,7 @@
       <c r="B25" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="14">
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -15547,7 +15766,7 @@
       <c r="O25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P25" s="15" t="s">
+      <c r="P25" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -15558,7 +15777,7 @@
       <c r="B26" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="14">
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -15597,7 +15816,7 @@
       <c r="O26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P26" s="15" t="s">
+      <c r="P26" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -15608,7 +15827,7 @@
       <c r="B27" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="14">
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -15647,7 +15866,7 @@
       <c r="O27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P27" s="15" t="s">
+      <c r="P27" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -15658,7 +15877,7 @@
       <c r="B28" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="14">
         <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -15697,7 +15916,7 @@
       <c r="O28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P28" s="15" t="s">
+      <c r="P28" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15708,7 +15927,7 @@
       <c r="B29" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="14">
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -15747,7 +15966,7 @@
       <c r="O29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P29" s="15" t="s">
+      <c r="P29" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15758,7 +15977,7 @@
       <c r="B30" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="14">
         <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -15797,7 +16016,7 @@
       <c r="O30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P30" s="15" t="s">
+      <c r="P30" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15808,7 +16027,7 @@
       <c r="B31" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="14">
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -15847,7 +16066,7 @@
       <c r="O31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P31" s="15" t="s">
+      <c r="P31" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15858,7 +16077,7 @@
       <c r="B32" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="14">
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -15897,7 +16116,7 @@
       <c r="O32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P32" s="15" t="s">
+      <c r="P32" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15908,7 +16127,7 @@
       <c r="B33" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="14">
         <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -15947,7 +16166,7 @@
       <c r="O33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P33" s="15" t="s">
+      <c r="P33" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15958,7 +16177,7 @@
       <c r="B34" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="14">
         <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -15997,7 +16216,7 @@
       <c r="O34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P34" s="15" t="s">
+      <c r="P34" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16008,7 +16227,7 @@
       <c r="B35" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="14">
         <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -16047,7 +16266,7 @@
       <c r="O35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P35" s="15" t="s">
+      <c r="P35" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16058,7 +16277,7 @@
       <c r="B36" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="14">
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -16097,7 +16316,7 @@
       <c r="O36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P36" s="15" t="s">
+      <c r="P36" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16108,7 +16327,7 @@
       <c r="B37" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="14">
         <v>4</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -16147,7 +16366,7 @@
       <c r="O37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P37" s="15" t="s">
+      <c r="P37" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16158,7 +16377,7 @@
       <c r="B38" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="14">
         <v>4</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -16197,7 +16416,7 @@
       <c r="O38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P38" s="15" t="s">
+      <c r="P38" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16208,7 +16427,7 @@
       <c r="B39" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="14">
         <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -16247,7 +16466,7 @@
       <c r="O39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P39" s="15" t="s">
+      <c r="P39" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16258,7 +16477,7 @@
       <c r="B40" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="14">
         <v>5</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -16297,7 +16516,7 @@
       <c r="O40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P40" s="15" t="s">
+      <c r="P40" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16308,7 +16527,7 @@
       <c r="B41" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="14">
         <v>5</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -16347,7 +16566,7 @@
       <c r="O41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P41" s="15" t="s">
+      <c r="P41" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16358,7 +16577,7 @@
       <c r="B42" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="14">
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -16397,7 +16616,7 @@
       <c r="O42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P42" s="15" t="s">
+      <c r="P42" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16408,7 +16627,7 @@
       <c r="B43" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43" s="14">
         <v>5</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -16447,7 +16666,7 @@
       <c r="O43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P43" s="15" t="s">
+      <c r="P43" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16458,7 +16677,7 @@
       <c r="B44" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="14">
         <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -16497,7 +16716,7 @@
       <c r="O44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P44" s="15" t="s">
+      <c r="P44" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16508,7 +16727,7 @@
       <c r="B45" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="14">
         <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -16547,7 +16766,7 @@
       <c r="O45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P45" s="15" t="s">
+      <c r="P45" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16558,7 +16777,7 @@
       <c r="B46" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C46" s="16">
+      <c r="C46" s="14">
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -16597,7 +16816,7 @@
       <c r="O46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P46" s="15" t="s">
+      <c r="P46" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16608,7 +16827,7 @@
       <c r="B47" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C47" s="16">
+      <c r="C47" s="14">
         <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -16647,7 +16866,7 @@
       <c r="O47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P47" s="15" t="s">
+      <c r="P47" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16658,7 +16877,7 @@
       <c r="B48" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="14">
         <v>9</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -16697,7 +16916,7 @@
       <c r="O48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P48" s="15" t="s">
+      <c r="P48" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16708,7 +16927,7 @@
       <c r="B49" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C49" s="14">
         <v>9</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -16747,7 +16966,7 @@
       <c r="O49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P49" s="15" t="s">
+      <c r="P49" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -16758,7 +16977,7 @@
       <c r="B50" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="14">
         <v>9</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -16797,7 +17016,7 @@
       <c r="O50" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P50" s="15" t="s">
+      <c r="P50" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -16859,7 +17078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACF069B-924A-40FE-91D9-4FC2DC64FE41}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -16900,7 +17119,7 @@
       <c r="B2" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -16920,7 +17139,7 @@
       <c r="B3" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -16940,7 +17159,7 @@
       <c r="B4" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -16960,7 +17179,7 @@
       <c r="B5" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -17000,7 +17219,7 @@
       <c r="B7" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -17040,7 +17259,7 @@
       <c r="B9" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -17060,7 +17279,7 @@
       <c r="B10" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>643</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -17139,7 +17358,7 @@
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>195</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -17157,16 +17376,16 @@
       <c r="G1" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>193</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>642</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="9" t="s">

</xml_diff>

<commit_message>
Add dogs to content lists
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D863C51E-4AB2-4110-9769-5C127DAF804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA701F21-72C3-4B6D-A2D1-0EEE751F4613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4687" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="799">
   <si>
     <t>Name</t>
   </si>
@@ -2439,6 +2439,42 @@
   </si>
   <si>
     <t>Spells</t>
+  </si>
+  <si>
+    <t>Small Dog</t>
+  </si>
+  <si>
+    <t>Medium Dog</t>
+  </si>
+  <si>
+    <t>Large Dog</t>
+  </si>
+  <si>
+    <t>Magic Dog Familiar</t>
+  </si>
+  <si>
+    <t>Magic Dog Steed</t>
+  </si>
+  <si>
+    <t>Dwarven Mine Dog</t>
+  </si>
+  <si>
+    <t>Elven Hunting Hound</t>
+  </si>
+  <si>
+    <t>Gnomish Trinket Retriever</t>
+  </si>
+  <si>
+    <t>Halfling Riding Mastiff</t>
+  </si>
+  <si>
+    <t>Celestial, Fey, or Fiend</t>
+  </si>
+  <si>
+    <t>Arctic, Coastal, Desert, Forest, Grassland, Hills, Jungle, Mountain, Swamp, Underdark, Urban</t>
+  </si>
+  <si>
+    <t>Dogs</t>
   </si>
 </sst>
 </file>
@@ -3724,11 +3760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J163"/>
+  <dimension ref="A1:J172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F161" sqref="F161"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8038,6 +8074,240 @@
         <v>16</v>
       </c>
     </row>
+    <row r="164" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C164" s="7">
+        <v>0</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E164" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C165" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E165" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C166" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E166" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C167" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E167" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C168" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E168" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C169" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E169" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C170" s="7">
+        <v>1</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E170" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C171" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E171" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C172" s="7">
+        <v>1</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E172" s="20" t="s">
+        <v>797</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I156" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A108:I156">
@@ -8045,7 +8315,7 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="G164:G1048576 G1:G141">
+  <conditionalFormatting sqref="G173:G1048576 G1:G141">
     <cfRule type="containsText" dxfId="101" priority="31" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",G1)))</formula>
     </cfRule>
@@ -8065,7 +8335,7 @@
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G142:G163">
+  <conditionalFormatting sqref="G142:G172">
     <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",G142)))</formula>
     </cfRule>
@@ -8213,9 +8483,11 @@
     <hyperlink ref="F158:F159" r:id="rId125" display="Wolves" xr:uid="{2C50CB26-3E8A-4828-A1B0-D4F70F9F7990}"/>
     <hyperlink ref="F160" r:id="rId126" xr:uid="{B906B306-9128-44E1-8E69-FC114E9C35E6}"/>
     <hyperlink ref="F161:F163" r:id="rId127" display="Werewolves" xr:uid="{8E85D40E-7B6E-4110-B17F-5A5F4B5A94F8}"/>
+    <hyperlink ref="F164" r:id="rId128" xr:uid="{0F4AE279-5A45-42DE-ADAB-EEBBFB7F5BB7}"/>
+    <hyperlink ref="F165:F172" r:id="rId129" display="Dogs" xr:uid="{D10EFFE4-4DDF-4DC7-BF44-FC58135E9A44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId128"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId130"/>
 </worksheet>
 </file>
 
@@ -8371,9 +8643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10383,8 +10655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E52FED-6497-4FDC-A0DA-7ECEAA0549B9}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add magic dogs to content list
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA701F21-72C3-4B6D-A2D1-0EEE751F4613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CF267B-7084-4073-8BD1-05FF8C8F392B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4782" uniqueCount="808">
   <si>
     <t>Name</t>
   </si>
@@ -2475,6 +2475,33 @@
   </si>
   <si>
     <t>Dogs</t>
+  </si>
+  <si>
+    <t>Bolt Hound</t>
+  </si>
+  <si>
+    <t>Flood Hound</t>
+  </si>
+  <si>
+    <t>Miniature Blink Dog</t>
+  </si>
+  <si>
+    <t>Aralez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemental </t>
+  </si>
+  <si>
+    <t>Chamrosh</t>
+  </si>
+  <si>
+    <t>Magic Dogs</t>
+  </si>
+  <si>
+    <t>Desert, Extraplanar, Mountain</t>
+  </si>
+  <si>
+    <t>Coastal, Extraplanar, Freshwater, Underwater</t>
   </si>
 </sst>
 </file>
@@ -2616,7 +2643,109 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="114">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3760,11 +3889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J172"/>
+  <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C172" sqref="C172"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,7 +3904,7 @@
     <col min="4" max="4" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -8308,6 +8437,127 @@
         <v>16</v>
       </c>
     </row>
+    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C173" s="7">
+        <v>1</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="E173" s="20" t="s">
+        <v>806</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C174" s="7">
+        <v>1</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="E174" s="20" t="s">
+        <v>807</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C175" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C176" s="7">
+        <v>3</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C177" s="7">
+        <v>6</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I156" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A108:I156">
@@ -8315,44 +8565,24 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="G173:G1048576 G1:G141">
-    <cfRule type="containsText" dxfId="101" priority="31" operator="containsText" text="Playtest Ready">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="32" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="33" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="34" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="35" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",G1)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="In Development">
+      <formula>NOT(ISERROR(SEARCH("In Development",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="36" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",G1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G142:G172">
-    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Playtest Ready">
-      <formula>NOT(ISERROR(SEARCH("Playtest Ready",G142)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",G142)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",G142)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Needs Clean Up">
-      <formula>NOT(ISERROR(SEARCH("Needs Clean Up",G142)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="In Development">
-      <formula>NOT(ISERROR(SEARCH("In Development",G142)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",G142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -8485,9 +8715,14 @@
     <hyperlink ref="F161:F163" r:id="rId127" display="Werewolves" xr:uid="{8E85D40E-7B6E-4110-B17F-5A5F4B5A94F8}"/>
     <hyperlink ref="F164" r:id="rId128" xr:uid="{0F4AE279-5A45-42DE-ADAB-EEBBFB7F5BB7}"/>
     <hyperlink ref="F165:F172" r:id="rId129" display="Dogs" xr:uid="{D10EFFE4-4DDF-4DC7-BF44-FC58135E9A44}"/>
+    <hyperlink ref="F173" r:id="rId130" xr:uid="{6C7332EE-3D6C-4441-B1A6-BC6AAF223A38}"/>
+    <hyperlink ref="F174" r:id="rId131" xr:uid="{878D497C-EB91-4390-920D-66DCEB5126F8}"/>
+    <hyperlink ref="F175" r:id="rId132" xr:uid="{2B3BD29E-A3B2-4429-A81E-C39B9C1AECC7}"/>
+    <hyperlink ref="F176" r:id="rId133" xr:uid="{C1836EEA-0C07-4F40-959F-ABAE2438B5AD}"/>
+    <hyperlink ref="F177" r:id="rId134" xr:uid="{802A0D9E-4007-4659-AC12-F4904512F62C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId130"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId135"/>
 </worksheet>
 </file>
 
@@ -8591,42 +8826,42 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{12EDD4A5-537C-4964-AE58-8E306F1BDAC3}"/>
   <conditionalFormatting sqref="D1 D4:D1048576">
-    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="40" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="38" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="37" priority="11" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8643,7 +8878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
@@ -10350,62 +10585,62 @@
   <autoFilter ref="A1:F1" xr:uid="{6F8015A8-CD76-4317-A710-EE332EB4DCD2}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B55 B58:B1048576">
-    <cfRule type="containsText" dxfId="17" priority="67" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="29" priority="67" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="68" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="28" priority="68" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="69" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="27" priority="69" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="70" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="26" priority="70" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="71" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="25" priority="71" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="72" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="24" priority="72" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",B56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B56)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10603,42 +10838,42 @@
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{8ECB4EEB-6E0F-4DBC-8ACA-83CFF1219E40}"/>
   <conditionalFormatting sqref="C1 C5:C1048576">
-    <cfRule type="containsText" dxfId="89" priority="13" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="101" priority="13" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="14" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="100" priority="14" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="15" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="99" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="16" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="98" priority="16" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="17" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="97" priority="17" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="18" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="96" priority="18" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="94" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10657,7 +10892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12734,22 +12969,22 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="86" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="In Development">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="In Development">
       <formula>NOT(ISERROR(SEARCH("In Development",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13780,22 +14015,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{DD42EE7F-9159-4C80-95B9-C05FE7C82AF2}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="80" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="78" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14712,22 +14947,22 @@
   <autoFilter ref="A1:G1" xr:uid="{75FD0084-15F3-4E8F-BDC9-AA450191B803}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17294,42 +17529,42 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="11" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17560,22 +17795,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20871,22 +21106,22 @@
   <autoFilter ref="A1:L69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21019,22 +21254,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Playtest Ready">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Needs Clean Up">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Needs Clean Up">
       <formula>NOT(ISERROR(SEARCH("Needs Clean Up",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Needs Review">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update content lists with kallikantzaros
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE05FF5-BBB5-416E-927D-3FE889134123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99C7EA0-98B0-4DEB-A70E-B1DA13983B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4782" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4796" uniqueCount="811">
   <si>
     <t>Name</t>
   </si>
@@ -2502,6 +2502,15 @@
   </si>
   <si>
     <t>Coastal, Extraplanar, Freshwater, Underwater</t>
+  </si>
+  <si>
+    <t>Kallikantzaros</t>
+  </si>
+  <si>
+    <t>Kallikantzaros Foreman</t>
+  </si>
+  <si>
+    <t>Extraplanar, Forest, Urban</t>
   </si>
 </sst>
 </file>
@@ -3736,11 +3745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J177"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8403,6 +8412,58 @@
       </c>
       <c r="H177" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C178" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E178" s="20" t="s">
+        <v>810</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C179" s="7">
+        <v>2</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E179" s="20" t="s">
+        <v>810</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -8567,9 +8628,11 @@
     <hyperlink ref="F175" r:id="rId132" xr:uid="{2B3BD29E-A3B2-4429-A81E-C39B9C1AECC7}"/>
     <hyperlink ref="F176" r:id="rId133" xr:uid="{C1836EEA-0C07-4F40-959F-ABAE2438B5AD}"/>
     <hyperlink ref="F177" r:id="rId134" xr:uid="{802A0D9E-4007-4659-AC12-F4904512F62C}"/>
+    <hyperlink ref="F178" r:id="rId135" xr:uid="{3F37297D-26ED-417D-9945-A82DAC56AB08}"/>
+    <hyperlink ref="F179" r:id="rId136" xr:uid="{E3C05C3E-9EBC-4092-BD0F-ED26019C6CFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId135"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId137"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add magic chariots to content lists
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99C7EA0-98B0-4DEB-A70E-B1DA13983B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6F986E-1EF5-4CAA-AC71-6793E3FCD4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4796" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4877" uniqueCount="824">
   <si>
     <t>Name</t>
   </si>
@@ -2511,6 +2511,45 @@
   </si>
   <si>
     <t>Extraplanar, Forest, Urban</t>
+  </si>
+  <si>
+    <t>Chariots</t>
+  </si>
+  <si>
+    <t>Orcish War Chariot</t>
+  </si>
+  <si>
+    <t>Scythed Chariot</t>
+  </si>
+  <si>
+    <t>Wagon</t>
+  </si>
+  <si>
+    <t>Sleigh</t>
+  </si>
+  <si>
+    <t>Small Wagon</t>
+  </si>
+  <si>
+    <t>War Chariot</t>
+  </si>
+  <si>
+    <t>Chariot</t>
+  </si>
+  <si>
+    <t>Burning Chariot</t>
+  </si>
+  <si>
+    <t>Chariot of The Seas</t>
+  </si>
+  <si>
+    <t>Chariot of The Wilds</t>
+  </si>
+  <si>
+    <t>Winged Chariot</t>
+  </si>
+  <si>
+    <t>Magic Chariots</t>
   </si>
 </sst>
 </file>
@@ -3747,7 +3786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F178" sqref="F178"/>
     </sheetView>
@@ -17487,10 +17526,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACF069B-924A-40FE-91D9-4FC2DC64FE41}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17703,8 +17742,129 @@
         <v>646</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D10">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="D1:D16">
     <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",D1)))</formula>
     </cfRule>
@@ -17734,6 +17894,8 @@
     <hyperlink ref="F4" r:id="rId7" display="New Weapons" xr:uid="{06D6BE93-4FE2-4532-A6F9-A86FF70D4EB6}"/>
     <hyperlink ref="F3" r:id="rId8" display="New Weapons" xr:uid="{307B2ED2-A702-4596-82DF-3468BA8704FF}"/>
     <hyperlink ref="F2" r:id="rId9" display="New Weapons" xr:uid="{CC9F76B0-4120-40E2-8D59-C8EC3C02CBCB}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{4E2A2B51-BBF2-4A61-B0B8-533F34EDDB66}"/>
+    <hyperlink ref="F12:F16" r:id="rId11" display="Chariots" xr:uid="{01020433-E409-4278-B2CE-83281F4A2DB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17741,11 +17903,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21010,6 +21172,134 @@
       </c>
       <c r="L98" s="3" t="s">
         <v>547</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L99" s="3" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L100" s="3" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L101" s="3" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>823</v>
       </c>
     </row>
   </sheetData>
@@ -21068,19 +21358,21 @@
     <hyperlink ref="L96" r:id="rId30" xr:uid="{ED811F94-656C-4B19-8082-13CCA6B82747}"/>
     <hyperlink ref="L97" r:id="rId31" xr:uid="{EC272C55-5424-4F1B-8102-5FB9A46D34BF}"/>
     <hyperlink ref="L98" r:id="rId32" xr:uid="{548B1A39-5B09-46AD-9A11-F3723B4EEC94}"/>
+    <hyperlink ref="L99" r:id="rId33" xr:uid="{A38D9E39-D067-48D2-AF89-4873B70B9371}"/>
+    <hyperlink ref="L100:L102" r:id="rId34" display="Magic Chariots" xr:uid="{707525D7-FDA6-40E2-B456-9DE15317972E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId35"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2F1729-7251-4389-9641-85685F236F2B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21159,6 +21451,23 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -21187,6 +21496,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BD2521FD-FF87-4C8B-99BE-7B21AA39FFD0}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{D4EA4825-1487-4570-B412-DF8E221C1BA1}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{7BFC501A-AD63-47FD-B8B6-597E83DED8A5}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{EA5696A4-BF5F-4647-B947-9A94FA6DA5EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add lore of light spells
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96508AE-EE4E-4986-B433-B0C258A6CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A6BBCA-40A6-4328-981E-EE8B014E898C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5376" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5584" uniqueCount="897">
   <si>
     <t>Name</t>
   </si>
@@ -2726,6 +2726,48 @@
   </si>
   <si>
     <t>Not on website</t>
+  </si>
+  <si>
+    <t>Cursed Blades</t>
+  </si>
+  <si>
+    <t>Decrepify</t>
+  </si>
+  <si>
+    <t>Guiding Wind</t>
+  </si>
+  <si>
+    <t>Incantation of Protection</t>
+  </si>
+  <si>
+    <t>Abjuration</t>
+  </si>
+  <si>
+    <t>Incantation of Zeal</t>
+  </si>
+  <si>
+    <t>Skull Storm</t>
+  </si>
+  <si>
+    <t>Tomb Strike</t>
+  </si>
+  <si>
+    <t>Burning Gaze</t>
+  </si>
+  <si>
+    <t>Dazzling Light</t>
+  </si>
+  <si>
+    <t>Holy Nova</t>
+  </si>
+  <si>
+    <t>Mass Haste</t>
+  </si>
+  <si>
+    <t>Net of Light</t>
+  </si>
+  <si>
+    <t>Warding Light</t>
   </si>
 </sst>
 </file>
@@ -15902,16 +15944,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
@@ -19065,6 +19107,695 @@
         <v>16</v>
       </c>
       <c r="Q62" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C63" s="14">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P63" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q63" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="14">
+        <v>4</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q64" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C65" s="14">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N65" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P65" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q65" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C66" s="14">
+        <v>2</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P66" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q66" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C67" s="14">
+        <v>2</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N67" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P67" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q67" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C68" s="14">
+        <v>6</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N68" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P68" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q68" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C69" s="14">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q69" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" s="14">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N70" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P70" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q70" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" s="14">
+        <v>3</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N71" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P71" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q71" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C72" s="14">
+        <v>4</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P72" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q72" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C73" s="14">
+        <v>8</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P73" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q73" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C74" s="14">
+        <v>4</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P74" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q74" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C75" s="14">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P75" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q75" s="13" t="s">
         <v>882</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add lore of shadow spells
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A6BBCA-40A6-4328-981E-EE8B014E898C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0A9CCC-8837-4869-B3FA-28281FC0E1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5584" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="905">
   <si>
     <t>Name</t>
   </si>
@@ -2768,6 +2768,30 @@
   </si>
   <si>
     <t>Warding Light</t>
+  </si>
+  <si>
+    <t>Mindrazors</t>
+  </si>
+  <si>
+    <t>Mirror Dance</t>
+  </si>
+  <si>
+    <t>Mystifying Miasma</t>
+  </si>
+  <si>
+    <t>Penumbral Pendulum</t>
+  </si>
+  <si>
+    <t>Pit of Shadows</t>
+  </si>
+  <si>
+    <t>Shroud of Dusk</t>
+  </si>
+  <si>
+    <t>Unseen Lurker</t>
+  </si>
+  <si>
+    <t>Withering Resolve</t>
   </si>
 </sst>
 </file>
@@ -8864,7 +8888,7 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="H170:H1048576 H1:H141">
+  <conditionalFormatting sqref="H1:H141 H170:H1048576">
     <cfRule type="containsText" dxfId="75" priority="35" operator="containsText" text="Needs Review">
       <formula>NOT(ISERROR(SEARCH("Needs Review",H1)))</formula>
     </cfRule>
@@ -15944,11 +15968,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19796,6 +19820,430 @@
         <v>16</v>
       </c>
       <c r="Q75" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C76" s="14">
+        <v>5</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P76" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q76" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C77" s="14">
+        <v>2</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P77" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q77" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78" s="14">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P78" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q78" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C79" s="14">
+        <v>4</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P79" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q79" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C80" s="14">
+        <v>6</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P80" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q80" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C81" s="14">
+        <v>1</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N81" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P81" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q81" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C82" s="14">
+        <v>3</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N82" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P82" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q82" s="13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C83" s="14">
+        <v>3</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N83" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P83" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q83" s="13" t="s">
         <v>882</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add lore of beasts spells
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A9AB6F-CE5D-41EA-8B92-2B33AB50804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC2734-6FB0-46EB-9640-E025C0F8D6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="841" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="841" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6586" uniqueCount="1064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6714" uniqueCount="1072">
   <si>
     <t>Name</t>
   </si>
@@ -3271,6 +3271,30 @@
   </si>
   <si>
     <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Amber Spear</t>
+  </si>
+  <si>
+    <t>Aspect of the Beast</t>
+  </si>
+  <si>
+    <t>Bestial Spirit</t>
+  </si>
+  <si>
+    <t>Call of the Pack</t>
+  </si>
+  <si>
+    <t>Impenetrable Pelt</t>
+  </si>
+  <si>
+    <t>Monstrous Transformation</t>
+  </si>
+  <si>
+    <t>Primal Dominance</t>
+  </si>
+  <si>
+    <t>Summon Flock</t>
   </si>
 </sst>
 </file>
@@ -19337,16 +19361,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
@@ -23613,6 +23637,430 @@
         <v>16</v>
       </c>
       <c r="Q83" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" s="14">
+        <v>3</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N84" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P84" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q84" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C85" s="14">
+        <v>4</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P85" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q85" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C86" s="14">
+        <v>4</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N86" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P86" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q86" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C87" s="14">
+        <v>5</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P87" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q87" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C88" s="14">
+        <v>5</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N88" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P88" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q88" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C89" s="14">
+        <v>6</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N89" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P89" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q89" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C90" s="14">
+        <v>2</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N90" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P90" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q90" s="13" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C91" s="14">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M91" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N91" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q91" s="13" t="s">
         <v>879</v>
       </c>
     </row>
@@ -27841,7 +28289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA41955-A4FB-4985-B786-1801358F3529}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>

</xml_diff>

<commit_message>
Add lore of the wild spells
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA72DB2-53EE-4C67-897C-8E80C2C7F582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C59F686-A2BC-475C-9681-BE0D8D88CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="841" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="841" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7640" uniqueCount="1233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7752" uniqueCount="1240">
   <si>
     <t>Name</t>
   </si>
@@ -3778,6 +3778,27 @@
   </si>
   <si>
     <t xml:space="preserve">The players face off against The Crone Grandmother, who resides within her monstrous crone's hut atop a hill in a forest clearing. </t>
+  </si>
+  <si>
+    <t>Bray Scream</t>
+  </si>
+  <si>
+    <t>Devolve</t>
+  </si>
+  <si>
+    <t>Mad Rampage</t>
+  </si>
+  <si>
+    <t>Mystic Signal</t>
+  </si>
+  <si>
+    <t>Savage Dominion</t>
+  </si>
+  <si>
+    <t>Traitor-Kin</t>
+  </si>
+  <si>
+    <t>Vile Tide</t>
   </si>
 </sst>
 </file>
@@ -4860,9 +4881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E253" sqref="E253"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G295" sqref="G295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22317,11 +22338,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C264C694-D993-4798-AD5F-1273142184DE}">
-  <dimension ref="A1:S98"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27388,6 +27409,377 @@
         <v>16</v>
       </c>
       <c r="Q98" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C99" s="14">
+        <v>3</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M99" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N99" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P99" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q99" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C100" s="14">
+        <v>1</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N100" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P100" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q100" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C101" s="14">
+        <v>4</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N101" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P101" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q101" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C102" s="14">
+        <v>5</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L102" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M102" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N102" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P102" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q102" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C103" s="14">
+        <v>7</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L103" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M103" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N103" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P103" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q103" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C104" s="14">
+        <v>3</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P104" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q104" s="13" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C105" s="14">
+        <v>2</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N105" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P105" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q105" s="13" t="s">
         <v>880</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Release lore of the wilds spells
</commit_message>
<xml_diff>
--- a/ContentList.xlsx
+++ b/ContentList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C59F686-A2BC-475C-9681-BE0D8D88CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9446CCB-2477-4B07-8C98-989681068F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="841" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7752" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7888" uniqueCount="1267">
   <si>
     <t>Name</t>
   </si>
@@ -3780,9 +3780,6 @@
     <t xml:space="preserve">The players face off against The Crone Grandmother, who resides within her monstrous crone's hut atop a hill in a forest clearing. </t>
   </si>
   <si>
-    <t>Bray Scream</t>
-  </si>
-  <si>
     <t>Devolve</t>
   </si>
   <si>
@@ -3799,6 +3796,90 @@
   </si>
   <si>
     <t>Vile Tide</t>
+  </si>
+  <si>
+    <t>Snack of Swiftness</t>
+  </si>
+  <si>
+    <t>Gingerbread Monsters</t>
+  </si>
+  <si>
+    <t>Shorthorn</t>
+  </si>
+  <si>
+    <t>Humandoid(Beastman)</t>
+  </si>
+  <si>
+    <t>Shorthorn Tormentor</t>
+  </si>
+  <si>
+    <t>Shorthorn Raider</t>
+  </si>
+  <si>
+    <t>Shorthorn Stalker</t>
+  </si>
+  <si>
+    <t>Longhorn</t>
+  </si>
+  <si>
+    <t>Longhorn Ravager</t>
+  </si>
+  <si>
+    <t>Besthorn</t>
+  </si>
+  <si>
+    <t>Besthorn Manripper</t>
+  </si>
+  <si>
+    <t>Warhorn</t>
+  </si>
+  <si>
+    <t>Beastlord</t>
+  </si>
+  <si>
+    <t>Beastman Compendium</t>
+  </si>
+  <si>
+    <t>Lesser Bray Shaman</t>
+  </si>
+  <si>
+    <t>Bray Shaman</t>
+  </si>
+  <si>
+    <t>Great Bray Shaman</t>
+  </si>
+  <si>
+    <t>Ginger Runner</t>
+  </si>
+  <si>
+    <t>Ginger Golem</t>
+  </si>
+  <si>
+    <t>Ginger Colossus</t>
+  </si>
+  <si>
+    <t>Extraplanar, Forest, Swamp, Urban</t>
+  </si>
+  <si>
+    <t>Ginger Creatures</t>
+  </si>
+  <si>
+    <t>The Dark Omen</t>
+  </si>
+  <si>
+    <t>Tomb Knight</t>
+  </si>
+  <si>
+    <t>Necropolis Serpent</t>
+  </si>
+  <si>
+    <t>Venom Knight</t>
+  </si>
+  <si>
+    <t>Tomb Knights</t>
+  </si>
+  <si>
+    <t>Primal Scream</t>
   </si>
 </sst>
 </file>
@@ -4879,11 +4960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K306"/>
+  <dimension ref="A1:K326"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G295" sqref="G295"/>
+      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D329" sqref="D329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13539,6 +13620,484 @@
       </c>
       <c r="I306" s="13" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C307" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E307" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F307" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H307" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I307" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C308" s="7">
+        <v>1</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E308" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F308" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H308" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I308" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C309" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E309" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F309" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H309" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I309" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C310" s="7">
+        <v>2</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E310" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F310" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H310" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I310" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A311" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C311" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E311" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F311" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H311" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I311" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C312" s="7">
+        <v>2</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E312" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F312" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H312" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I312" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C313" s="7">
+        <v>2</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E313" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F313" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H313" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I313" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C314" s="7">
+        <v>4</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E314" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F314" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H314" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I314" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C315" s="7">
+        <v>6</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E315" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F315" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H315" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I315" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C316" s="7">
+        <v>9</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E316" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F316" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H316" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I316" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C317" s="7">
+        <v>3</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E317" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F317" s="3" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C318" s="7">
+        <v>6</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E318" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F318" s="3" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A319" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C319" s="7">
+        <v>9</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E319" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F319" s="3" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C320" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E320" s="20" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F320" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="H320" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I320" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C321" s="7">
+        <v>4</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E321" s="20" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F321" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="H321" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I321" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C322" s="7">
+        <v>11</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E322" s="20" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F322" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="H322" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I322" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C323" s="7">
+        <v>16</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E323" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="F323" s="3" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C324" s="7">
+        <v>5</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E324" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="F324" s="3" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C325" s="7">
+        <v>2</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E325" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="F325" s="3" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C326" s="7">
+        <v>4</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E326" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="F326" s="3" t="s">
+        <v>1265</v>
       </c>
     </row>
   </sheetData>
@@ -13937,9 +14496,19 @@
     <hyperlink ref="F304" r:id="rId356" location="p16" xr:uid="{49BCC511-2DD2-480A-A0E8-C83615ABFD1B}"/>
     <hyperlink ref="F305" r:id="rId357" location="p16" xr:uid="{F9D1066A-8CBC-4306-AD11-623074ECEAB2}"/>
     <hyperlink ref="F306" r:id="rId358" location="p16" xr:uid="{D4B20E9B-98EF-4BCC-AC93-6F331EEE7D4C}"/>
+    <hyperlink ref="F307" r:id="rId359" xr:uid="{7D8722E1-0D82-4A75-BA69-53033C9F5A5C}"/>
+    <hyperlink ref="F308:F316" r:id="rId360" display="Beastman Compendium" xr:uid="{9D81826C-1B4C-41A3-AE23-767E665F20DF}"/>
+    <hyperlink ref="F317" r:id="rId361" xr:uid="{FA9AC2DC-B9C3-485F-94C6-C94281BEDE34}"/>
+    <hyperlink ref="F318" r:id="rId362" xr:uid="{68A7530C-37F1-44BE-A127-D100E8FB1B11}"/>
+    <hyperlink ref="F319" r:id="rId363" xr:uid="{F4F099A6-CD54-4600-9530-090F2690CB9B}"/>
+    <hyperlink ref="F320" r:id="rId364" xr:uid="{5DCE34FF-015E-4D4C-9931-1521063E153A}"/>
+    <hyperlink ref="F321:F322" r:id="rId365" display="Ginger Creatures" xr:uid="{DE69B376-DB5E-4D83-A3BA-5B4D8B3A50E7}"/>
+    <hyperlink ref="F323" r:id="rId366" xr:uid="{4E0E3B95-46F8-49E2-A1EE-C6711FC2850B}"/>
+    <hyperlink ref="F324" r:id="rId367" xr:uid="{86BE1E30-0D6B-409A-AE8F-8E8E55EEC10D}"/>
+    <hyperlink ref="F325:F326" r:id="rId368" display="Tomb Knights" xr:uid="{A0EF2C37-4ED5-47E7-8702-E602A90FFDE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId359"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId369"/>
 </worksheet>
 </file>
 
@@ -16171,7 +16740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>826</v>
       </c>
@@ -16188,7 +16757,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>835</v>
       </c>
@@ -16205,7 +16774,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>860</v>
       </c>
@@ -16222,7 +16791,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>859</v>
       </c>
@@ -22342,7 +22911,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
+      <selection pane="bottomLeft" activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27414,7 +27983,7 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>1233</v>
+        <v>1266</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>262</v>
@@ -27453,7 +28022,7 @@
         <v>24</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O99" s="1" t="s">
         <v>14</v>
@@ -27467,7 +28036,7 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>262</v>
@@ -27506,7 +28075,7 @@
         <v>24</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O100" s="1" t="s">
         <v>14</v>
@@ -27520,7 +28089,7 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>262</v>
@@ -27559,7 +28128,7 @@
         <v>24</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O101" s="1" t="s">
         <v>14</v>
@@ -27573,7 +28142,7 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>262</v>
@@ -27612,7 +28181,7 @@
         <v>40</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O102" s="1" t="s">
         <v>14</v>
@@ -27626,7 +28195,7 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>262</v>
@@ -27665,7 +28234,7 @@
         <v>24</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O103" s="1" t="s">
         <v>14</v>
@@ -27679,7 +28248,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>262</v>
@@ -27718,7 +28287,7 @@
         <v>24</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O104" s="1" t="s">
         <v>14</v>
@@ -27732,7 +28301,7 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>262</v>
@@ -27771,7 +28340,7 @@
         <v>24</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O105" s="1" t="s">
         <v>14</v>
@@ -28219,11 +28788,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32137,6 +32706,41 @@
         <v>846</v>
       </c>
     </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D118" s="24">
+        <v>200</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L118" s="3" t="s">
+        <v>1240</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L69" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L98">
@@ -32148,8 +32752,8 @@
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Playtest Ready">
       <formula>NOT(ISERROR(SEARCH("Playtest Ready",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="Needs Review">
-      <formula>NOT(ISERROR(SEARCH("Needs Review",J1)))</formula>
+    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="In Development">
+      <formula>NOT(ISERROR(SEARCH("In Development",J1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J1)))</formula>
@@ -32215,9 +32819,10 @@
     <hyperlink ref="L115" r:id="rId48" location="p16" xr:uid="{C029E2CE-923A-4B62-B54A-B6FF561E617E}"/>
     <hyperlink ref="L116" r:id="rId49" location="p16" xr:uid="{C2508372-7C14-4C7B-BA4A-0226F00ACA9D}"/>
     <hyperlink ref="L117" r:id="rId50" location="p16" xr:uid="{13157784-996E-48C9-A6AA-1A61F0C2763F}"/>
+    <hyperlink ref="L118" r:id="rId51" xr:uid="{5E41288B-0C2A-4FA4-9C02-4AEDABE287A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId51"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId52"/>
 </worksheet>
 </file>
 
@@ -32246,7 +32851,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>

</xml_diff>